<commit_message>
feat(llm): benchmark data prep
</commit_message>
<xml_diff>
--- a/BogoInsight/crawlers/llm_additional_data.xlsx
+++ b/BogoInsight/crawlers/llm_additional_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ai\BogoInsight\BogoInsight\crawlers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DC53916B-6891-46F5-8D42-3060B6D4D506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80C0B05-102E-40B3-AA3E-44D8DC7DFE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0BF4306-33E7-4D31-A9A6-85483F972F05}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="118">
   <si>
     <t>name</t>
   </si>
@@ -97,9 +97,6 @@
     <t>PaLM</t>
   </si>
   <si>
-    <t>GPT-3.5 Turbo</t>
-  </si>
-  <si>
     <t>Claude</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
   </si>
   <si>
     <t>Meta</t>
-  </si>
-  <si>
-    <t>GPT-3.5 Turbo 0301</t>
   </si>
   <si>
     <t>Huawei</t>
@@ -382,6 +376,36 @@
   </si>
   <si>
     <t>GPT-4o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Llama 2 7B</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DROP</t>
+  </si>
+  <si>
+    <t>HumanEval</t>
+  </si>
+  <si>
+    <t>MATH</t>
+  </si>
+  <si>
+    <t>MMLU</t>
+  </si>
+  <si>
+    <t>MMMU</t>
+  </si>
+  <si>
+    <t>MathVista</t>
+  </si>
+  <si>
+    <t>GPT-3.5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPT-3.5 Turbo 0301</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1373,13 +1397,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFF9F69-317C-4CBC-86A8-E43FD4E7E879}">
-  <dimension ref="A1:O89"/>
+  <dimension ref="A1:U90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="R56" sqref="R56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1398,9 +1422,11 @@
     <col min="12" max="12" width="10.88671875" customWidth="1"/>
     <col min="13" max="13" width="10.6640625" customWidth="1"/>
     <col min="14" max="14" width="10.44140625" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1441,13 +1467,31 @@
         <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1459,7 +1503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -1474,7 +1518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1489,9 +1533,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>116</v>
       </c>
       <c r="B5" s="1">
         <v>44893</v>
@@ -1521,9 +1565,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="B6" s="1">
         <v>44986</v>
@@ -1549,10 +1593,25 @@
       <c r="K6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L6" t="b">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>70</v>
+      </c>
+      <c r="Q6">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="R6">
+        <v>48.1</v>
+      </c>
+      <c r="S6">
+        <v>34.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1">
         <v>45090</v>
@@ -1579,9 +1638,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1">
         <v>45236</v>
@@ -1608,9 +1667,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B9" s="1">
         <v>45316</v>
@@ -1640,9 +1699,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1">
         <v>44999</v>
@@ -1668,10 +1727,22 @@
       <c r="K10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <v>86.4</v>
+      </c>
+      <c r="Q10">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="R10">
+        <v>67</v>
+      </c>
+      <c r="S10">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1">
         <v>44999</v>
@@ -1701,9 +1772,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1">
         <v>45090</v>
@@ -1730,9 +1801,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1">
         <v>45090</v>
@@ -1759,9 +1830,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1">
         <v>45194</v>
@@ -1797,9 +1868,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1">
         <v>45236</v>
@@ -1825,10 +1896,22 @@
       <c r="K15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15">
+        <v>86.5</v>
+      </c>
+      <c r="Q15">
+        <v>86</v>
+      </c>
+      <c r="R15">
+        <v>87.1</v>
+      </c>
+      <c r="S15">
+        <v>72.599999999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" s="1">
         <v>45316</v>
@@ -1855,9 +1938,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B17" s="1">
         <v>45391</v>
@@ -1892,10 +1975,16 @@
       <c r="N17" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="T17">
+        <v>63.1</v>
+      </c>
+      <c r="U17">
+        <v>58.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B18" s="1">
         <v>45425</v>
@@ -1904,7 +1993,7 @@
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E18">
         <v>128</v>
@@ -1933,8 +2022,26 @@
       <c r="N18" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <v>88.7</v>
+      </c>
+      <c r="Q18">
+        <v>83.4</v>
+      </c>
+      <c r="R18">
+        <v>90.2</v>
+      </c>
+      <c r="S18">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="T18">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="U18">
+        <v>63.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -1949,7 +2056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1964,7 +2071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -1979,7 +2086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -1994,9 +2101,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1">
         <v>45056</v>
@@ -2023,9 +2130,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B24" s="1">
         <v>45343</v>
@@ -2048,16 +2155,25 @@
       <c r="L24" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P24">
+        <v>64.3</v>
+      </c>
+      <c r="R24">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="S24">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B25" s="1">
         <v>45426</v>
       </c>
       <c r="C25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D25">
         <v>27</v>
@@ -2080,16 +2196,19 @@
       <c r="M25" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B26" s="1">
         <v>45426</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -2122,15 +2241,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B27" s="1">
         <v>45283</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D27">
         <v>1600</v>
@@ -2165,16 +2284,34 @@
       <c r="O27" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P27">
+        <v>71.8</v>
+      </c>
+      <c r="Q27">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="R27">
+        <v>67.7</v>
+      </c>
+      <c r="S27">
+        <v>32.6</v>
+      </c>
+      <c r="T27">
+        <v>47.9</v>
+      </c>
+      <c r="U27">
+        <v>46.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B28" s="1">
         <v>45283</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D28">
         <v>100</v>
@@ -2194,19 +2331,31 @@
       <c r="O28" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P28">
+        <v>58.8</v>
+      </c>
+      <c r="S28">
+        <v>22.8</v>
+      </c>
+      <c r="T28">
+        <v>32.6</v>
+      </c>
+      <c r="U28">
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B29" s="1">
         <v>45330</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E29">
         <v>91.727999999999994</v>
@@ -2226,19 +2375,37 @@
       <c r="O29" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P29">
+        <v>83.7</v>
+      </c>
+      <c r="Q29">
+        <v>82.4</v>
+      </c>
+      <c r="R29">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="S29">
+        <v>53.2</v>
+      </c>
+      <c r="T29">
+        <v>59.4</v>
+      </c>
+      <c r="U29">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B30" s="1">
         <v>45337</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E30">
         <v>1000</v>
@@ -2267,19 +2434,37 @@
       <c r="O30" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P30">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="Q30">
+        <v>83.5</v>
+      </c>
+      <c r="R30">
+        <v>84.1</v>
+      </c>
+      <c r="S30">
+        <v>58.5</v>
+      </c>
+      <c r="T30">
+        <v>58.5</v>
+      </c>
+      <c r="U30">
+        <v>54.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B31" s="1">
         <v>45426</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E31">
         <v>2000</v>
@@ -2308,19 +2493,37 @@
       <c r="O31" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P31">
+        <v>85.9</v>
+      </c>
+      <c r="Q31">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="R31">
+        <v>84.1</v>
+      </c>
+      <c r="S31">
+        <v>67.7</v>
+      </c>
+      <c r="T31">
+        <v>62.2</v>
+      </c>
+      <c r="U31">
+        <v>63.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B32" s="1">
         <v>45426</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E32">
         <v>1000</v>
@@ -2346,10 +2549,28 @@
       <c r="O32" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P32">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="Q32">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="R32">
+        <v>74.3</v>
+      </c>
+      <c r="S32">
+        <v>54.9</v>
+      </c>
+      <c r="T32">
+        <v>56.1</v>
+      </c>
+      <c r="U32">
+        <v>58.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B33" s="1"/>
       <c r="D33">
@@ -2365,15 +2586,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B34" s="1">
         <v>45125</v>
       </c>
       <c r="C34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D34">
         <v>70</v>
@@ -2394,7 +2615,7 @@
         <v>2000</v>
       </c>
       <c r="K34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L34" t="b">
         <v>1</v>
@@ -2402,16 +2623,28 @@
       <c r="M34" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P34">
+        <v>69.7</v>
+      </c>
+      <c r="Q34">
+        <v>70.2</v>
+      </c>
+      <c r="R34">
+        <v>25.6</v>
+      </c>
+      <c r="S34">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B35" s="1">
         <v>45125</v>
       </c>
       <c r="C35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D35">
         <v>13</v>
@@ -2432,53 +2665,77 @@
         <v>2000</v>
       </c>
       <c r="K35" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="P35">
+        <v>53.8</v>
+      </c>
+      <c r="Q35">
+        <v>49.8</v>
+      </c>
+      <c r="R35">
+        <v>14</v>
+      </c>
+      <c r="S35">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="B36" s="1">
-        <v>45400</v>
+        <v>45125</v>
       </c>
       <c r="C36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D36">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E36">
-        <v>8.1920000000000002</v>
+        <v>4.0960000000000001</v>
       </c>
       <c r="F36">
-        <v>8.1920000000000002</v>
+        <v>4.0960000000000001</v>
       </c>
       <c r="G36">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H36">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="J36">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="K36" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="P36">
+        <v>45.7</v>
+      </c>
+      <c r="Q36">
+        <v>37.9</v>
+      </c>
+      <c r="R36">
+        <v>7.9</v>
+      </c>
+      <c r="S36">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B37" s="1">
         <v>45400</v>
       </c>
       <c r="C37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D37">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="E37">
         <v>8.1920000000000002</v>
@@ -2487,65 +2744,86 @@
         <v>8.1920000000000002</v>
       </c>
       <c r="G37">
-        <v>0.59</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H37">
-        <v>0.79</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J37">
         <v>15000</v>
       </c>
       <c r="K37" t="s">
-        <v>78</v>
-      </c>
-      <c r="L37" t="b">
-        <v>1</v>
-      </c>
-      <c r="M37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="P37">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="Q37">
+        <v>58.4</v>
+      </c>
+      <c r="R37">
+        <v>62.2</v>
+      </c>
+      <c r="S37">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="B38" s="1">
+        <v>45400</v>
+      </c>
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38">
+        <v>70</v>
+      </c>
+      <c r="E38">
+        <v>8.1920000000000002</v>
+      </c>
+      <c r="F38">
+        <v>8.1920000000000002</v>
+      </c>
+      <c r="G38">
+        <v>0.59</v>
+      </c>
+      <c r="H38">
+        <v>0.79</v>
+      </c>
+      <c r="J38">
+        <v>15000</v>
+      </c>
+      <c r="K38" t="s">
+        <v>76</v>
+      </c>
+      <c r="L38" t="b">
+        <v>1</v>
+      </c>
+      <c r="M38" t="b">
+        <v>1</v>
+      </c>
+      <c r="P38">
+        <v>79.5</v>
+      </c>
+      <c r="Q38">
+        <v>79.7</v>
+      </c>
+      <c r="R38">
+        <v>81.7</v>
+      </c>
+      <c r="S38">
+        <v>50.4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="1">
         <v>44893</v>
-      </c>
-      <c r="E38">
-        <v>100</v>
-      </c>
-      <c r="F38">
-        <v>4.0960000000000001</v>
-      </c>
-      <c r="G38">
-        <v>8</v>
-      </c>
-      <c r="H38">
-        <v>24</v>
-      </c>
-      <c r="J38">
-        <v>400</v>
-      </c>
-      <c r="K38" t="s">
-        <v>27</v>
-      </c>
-      <c r="L38" t="b">
-        <v>1</v>
-      </c>
-      <c r="M38" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" s="1">
-        <v>45118</v>
-      </c>
-      <c r="D39" t="s">
-        <v>85</v>
       </c>
       <c r="E39">
         <v>100</v>
@@ -2559,6 +2837,12 @@
       <c r="H39">
         <v>24</v>
       </c>
+      <c r="J39">
+        <v>400</v>
+      </c>
+      <c r="K39" t="s">
+        <v>26</v>
+      </c>
       <c r="L39" t="b">
         <v>1</v>
       </c>
@@ -2566,18 +2850,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B40" s="1">
-        <v>45253</v>
+        <v>45118</v>
       </c>
       <c r="D40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E40">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F40">
         <v>4.0960000000000001</v>
@@ -2594,16 +2878,22 @@
       <c r="M40" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P40">
+        <v>75</v>
+      </c>
+      <c r="R40">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="B41" s="1">
-        <v>45355</v>
+        <v>45253</v>
       </c>
       <c r="D41" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E41">
         <v>200</v>
@@ -2612,27 +2902,27 @@
         <v>4.0960000000000001</v>
       </c>
       <c r="G41">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H41">
-        <v>15</v>
-      </c>
-      <c r="I41">
-        <v>4.8</v>
-      </c>
-      <c r="N41" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="L41" t="b">
+        <v>1</v>
+      </c>
+      <c r="M41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B42" s="1">
         <v>45355</v>
       </c>
       <c r="D42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E42">
         <v>200</v>
@@ -2641,27 +2931,51 @@
         <v>4.0960000000000001</v>
       </c>
       <c r="G42">
-        <v>15</v>
+        <v>0.25</v>
       </c>
       <c r="H42">
-        <v>75</v>
+        <v>1.25</v>
       </c>
       <c r="I42">
-        <v>24</v>
+        <v>0.4</v>
+      </c>
+      <c r="L42" t="b">
+        <v>1</v>
+      </c>
+      <c r="M42" t="b">
+        <v>1</v>
       </c>
       <c r="N42" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P42">
+        <v>75.2</v>
+      </c>
+      <c r="Q42">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="R42">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="S42">
+        <v>38.9</v>
+      </c>
+      <c r="T42">
+        <v>50.2</v>
+      </c>
+      <c r="U42">
+        <v>46.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B43" s="1">
         <v>45355</v>
       </c>
       <c r="D43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E43">
         <v>200</v>
@@ -2670,155 +2984,206 @@
         <v>4.0960000000000001</v>
       </c>
       <c r="G43">
-        <v>0.25</v>
+        <v>3</v>
       </c>
       <c r="H43">
-        <v>1.25</v>
+        <v>15</v>
       </c>
       <c r="I43">
-        <v>0.4</v>
-      </c>
-      <c r="L43" t="b">
-        <v>1</v>
-      </c>
-      <c r="M43" t="b">
-        <v>1</v>
+        <v>4.8</v>
       </c>
       <c r="N43" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P43">
+        <v>79</v>
+      </c>
+      <c r="Q43">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="R43">
+        <v>73</v>
+      </c>
+      <c r="S43">
+        <v>43.1</v>
+      </c>
+      <c r="T43">
+        <v>53.1</v>
+      </c>
+      <c r="U43">
+        <v>47.9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B44" s="1">
-        <v>45141</v>
-      </c>
-      <c r="C44" t="s">
-        <v>44</v>
-      </c>
-      <c r="D44">
-        <v>7</v>
+        <v>45355</v>
+      </c>
+      <c r="D44" t="s">
+        <v>80</v>
       </c>
       <c r="E44">
-        <v>6</v>
+        <v>200</v>
       </c>
       <c r="F44">
-        <v>2</v>
+        <v>4.0960000000000001</v>
       </c>
       <c r="G44">
-        <v>0.85</v>
+        <v>15</v>
       </c>
       <c r="H44">
-        <v>0.85</v>
-      </c>
-      <c r="K44" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="I44">
+        <v>24</v>
+      </c>
+      <c r="N44" t="b">
+        <v>1</v>
+      </c>
+      <c r="P44">
+        <v>86.8</v>
+      </c>
+      <c r="Q44">
+        <v>83.1</v>
+      </c>
+      <c r="R44">
+        <v>84.9</v>
+      </c>
+      <c r="S44">
+        <v>60.1</v>
+      </c>
+      <c r="T44">
+        <v>59.4</v>
+      </c>
+      <c r="U44">
+        <v>50.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B45" s="1">
-        <v>45194</v>
+        <v>45260</v>
       </c>
       <c r="C45" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D45">
-        <v>14</v>
+        <v>1.8</v>
       </c>
       <c r="E45">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F45">
         <v>2</v>
       </c>
       <c r="G45">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="H45">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="K45" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="P45">
+        <v>45.3</v>
+      </c>
+      <c r="R45">
+        <v>15.2</v>
+      </c>
+      <c r="S45">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B46" s="1">
-        <v>45260</v>
+        <v>45141</v>
       </c>
       <c r="C46" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D46">
-        <v>1.8</v>
+        <v>7</v>
       </c>
       <c r="E46">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="F46">
         <v>2</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="K46" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="P46">
+        <v>58.2</v>
+      </c>
+      <c r="R46">
+        <v>31.6</v>
+      </c>
+      <c r="S46">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B47" s="1">
-        <v>45260</v>
+        <v>45194</v>
       </c>
       <c r="C47" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D47">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="E47">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="F47">
         <v>2</v>
       </c>
       <c r="G47">
-        <v>2.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H47">
-        <v>2.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K47" t="s">
-        <v>45</v>
-      </c>
-      <c r="L47" t="b">
-        <v>1</v>
-      </c>
-      <c r="M47" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="P47">
+        <v>66.3</v>
+      </c>
+      <c r="R47">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="S47">
+        <v>24.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B48" s="1">
-        <v>45328</v>
+        <v>45260</v>
       </c>
       <c r="C48" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D48">
         <v>72</v>
@@ -2836,42 +3201,63 @@
         <v>2.8</v>
       </c>
       <c r="K48" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L48" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M48" t="b">
+        <v>1</v>
+      </c>
+      <c r="P48">
+        <v>77.400000000000006</v>
+      </c>
+      <c r="R48">
+        <v>52.2</v>
+      </c>
+      <c r="S48">
+        <v>35.200000000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B49" s="1">
         <v>45328</v>
       </c>
       <c r="C49" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D49">
-        <v>7</v>
+        <v>0.5</v>
       </c>
       <c r="E49">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F49">
         <v>2</v>
       </c>
       <c r="G49">
-        <v>0.85</v>
+        <v>0</v>
       </c>
       <c r="H49">
-        <v>0.85</v>
+        <v>0</v>
       </c>
       <c r="K49" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="P49">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="R49">
+        <v>12.2</v>
+      </c>
+      <c r="S49">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>65</v>
       </c>
@@ -2879,10 +3265,10 @@
         <v>45328</v>
       </c>
       <c r="C50" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D50">
-        <v>32</v>
+        <v>1.8</v>
       </c>
       <c r="E50">
         <v>30</v>
@@ -2897,21 +3283,30 @@
         <v>0</v>
       </c>
       <c r="K50" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="P50">
+        <v>46.8</v>
+      </c>
+      <c r="R50">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="S50">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B51" s="1">
         <v>45328</v>
       </c>
       <c r="C51" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D51">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E51">
         <v>6</v>
@@ -2920,56 +3315,74 @@
         <v>2</v>
       </c>
       <c r="G51">
-        <v>1.1000000000000001</v>
+        <v>0.85</v>
       </c>
       <c r="H51">
-        <v>1.1000000000000001</v>
+        <v>0.85</v>
       </c>
       <c r="K51" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="P51">
+        <v>61</v>
+      </c>
+      <c r="R51">
+        <v>36</v>
+      </c>
+      <c r="S51">
+        <v>20.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B52" s="1">
         <v>45328</v>
       </c>
       <c r="C52" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D52">
-        <v>1.8</v>
+        <v>14</v>
       </c>
       <c r="E52">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="F52">
         <v>2</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H52">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K52" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="P52">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="R52">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="S52">
+        <v>29.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B53" s="1">
         <v>45328</v>
       </c>
       <c r="C53" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D53">
-        <v>0.5</v>
+        <v>32</v>
       </c>
       <c r="E53">
         <v>30</v>
@@ -2984,21 +3397,30 @@
         <v>0</v>
       </c>
       <c r="K53" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="P53">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="R53">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="S53">
+        <v>36.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B54" s="1">
-        <v>45402</v>
+        <v>45328</v>
       </c>
       <c r="C54" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D54">
-        <v>110</v>
+        <v>72</v>
       </c>
       <c r="E54">
         <v>30</v>
@@ -3007,106 +3429,121 @@
         <v>2</v>
       </c>
       <c r="G54">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="H54">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="K54" t="s">
-        <v>45</v>
-      </c>
-      <c r="M54" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="L54" t="b">
+        <v>1</v>
+      </c>
+      <c r="P54">
+        <v>77.5</v>
+      </c>
+      <c r="R54">
+        <v>41.5</v>
+      </c>
+      <c r="S54">
+        <v>34.1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="B55" s="1">
-        <v>45027</v>
+        <v>45402</v>
       </c>
       <c r="C55" t="s">
-        <v>44</v>
-      </c>
-      <c r="D55" t="s">
-        <v>109</v>
+        <v>42</v>
+      </c>
+      <c r="D55">
+        <v>110</v>
       </c>
       <c r="E55">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F55">
         <v>2</v>
       </c>
       <c r="G55">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="H55">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="K55" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="M55" t="b">
+        <v>1</v>
+      </c>
+      <c r="P55">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="R55">
+        <v>52.4</v>
+      </c>
+      <c r="S55">
+        <v>49.6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B56" s="1">
         <v>45027</v>
       </c>
       <c r="C56" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D56" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E56">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="F56">
         <v>2</v>
       </c>
       <c r="G56">
-        <v>2.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H56">
-        <v>2.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K56" t="s">
         <v>20</v>
       </c>
-      <c r="L56" t="b">
-        <v>1</v>
-      </c>
-      <c r="M56" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B57" s="1">
-        <v>45261</v>
+        <v>45027</v>
       </c>
       <c r="C57" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D57" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E57">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F57">
         <v>2</v>
       </c>
       <c r="G57">
-        <v>16.600000000000001</v>
+        <v>2.8</v>
       </c>
       <c r="H57">
-        <v>16.600000000000001</v>
+        <v>2.8</v>
       </c>
       <c r="K57" t="s">
         <v>20</v>
@@ -3114,19 +3551,22 @@
       <c r="L57" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B58" s="1">
-        <v>45298</v>
+        <v>45261</v>
       </c>
       <c r="C58" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D58" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E58">
         <v>6</v>
@@ -3143,19 +3583,22 @@
       <c r="K58" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B59" s="1">
-        <v>45385</v>
+        <v>45298</v>
       </c>
       <c r="C59" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D59" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E59">
         <v>6</v>
@@ -3172,22 +3615,19 @@
       <c r="K59" t="s">
         <v>20</v>
       </c>
-      <c r="M59" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B60" s="1">
-        <v>45410</v>
+        <v>45385</v>
       </c>
       <c r="C60" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D60" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E60">
         <v>6</v>
@@ -3204,25 +3644,22 @@
       <c r="K60" t="s">
         <v>20</v>
       </c>
-      <c r="L60" t="b">
-        <v>1</v>
-      </c>
       <c r="M60" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B61" s="1">
-        <v>45261</v>
+        <v>45410</v>
       </c>
       <c r="C61" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D61" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E61">
         <v>6</v>
@@ -3231,30 +3668,33 @@
         <v>2</v>
       </c>
       <c r="G61">
-        <v>1.1000000000000001</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="H61">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I61">
-        <v>1.4</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="K61" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L61" t="b">
+        <v>1</v>
+      </c>
+      <c r="M61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B62" s="1">
         <v>45261</v>
       </c>
       <c r="C62" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D62" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E62">
         <v>6</v>
@@ -3263,59 +3703,65 @@
         <v>2</v>
       </c>
       <c r="G62">
-        <v>2.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H62">
-        <v>2.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I62">
-        <v>3.6</v>
+        <v>1.4</v>
       </c>
       <c r="K62" t="s">
         <v>20</v>
       </c>
-      <c r="L62" t="b">
-        <v>1</v>
-      </c>
-      <c r="M62" t="b">
-        <v>1</v>
-      </c>
-      <c r="N62" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>48</v>
+        <v>106</v>
       </c>
       <c r="B63" s="1">
+        <v>45261</v>
+      </c>
+      <c r="C63" t="s">
+        <v>42</v>
+      </c>
+      <c r="D63" t="s">
+        <v>101</v>
+      </c>
+      <c r="E63">
+        <v>6</v>
+      </c>
+      <c r="F63">
+        <v>2</v>
+      </c>
+      <c r="G63">
+        <v>2.8</v>
+      </c>
+      <c r="H63">
+        <v>2.8</v>
+      </c>
+      <c r="I63">
+        <v>3.6</v>
+      </c>
+      <c r="K63" t="s">
+        <v>20</v>
+      </c>
+      <c r="L63" t="b">
+        <v>1</v>
+      </c>
+      <c r="M63" t="b">
+        <v>1</v>
+      </c>
+      <c r="N63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B64" s="1">
         <v>45196</v>
-      </c>
-      <c r="E63">
-        <v>32.768000000000001</v>
-      </c>
-      <c r="F63">
-        <v>32.768000000000001</v>
-      </c>
-      <c r="G63">
-        <v>0</v>
-      </c>
-      <c r="H63">
-        <v>0</v>
-      </c>
-      <c r="L63" t="b">
-        <v>1</v>
-      </c>
-      <c r="M63" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B64" s="1">
-        <v>45271</v>
       </c>
       <c r="E64">
         <v>32.768000000000001</v>
@@ -3324,46 +3770,37 @@
         <v>32.768000000000001</v>
       </c>
       <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="L64" t="b">
+        <v>1</v>
+      </c>
+      <c r="M64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B65" s="1">
+        <v>45271</v>
+      </c>
+      <c r="E65">
+        <v>32.768000000000001</v>
+      </c>
+      <c r="F65">
+        <v>32.768000000000001</v>
+      </c>
+      <c r="G65">
         <v>0.24</v>
       </c>
-      <c r="H64">
+      <c r="H65">
         <v>0.24</v>
       </c>
-      <c r="L64" t="b">
-        <v>1</v>
-      </c>
-      <c r="M64" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B65" s="1">
-        <v>45348</v>
-      </c>
-      <c r="C65" t="s">
-        <v>83</v>
-      </c>
-      <c r="D65" t="s">
-        <v>84</v>
-      </c>
-      <c r="E65">
-        <v>32</v>
-      </c>
-      <c r="F65">
-        <v>32</v>
-      </c>
-      <c r="G65">
-        <v>8</v>
-      </c>
-      <c r="H65">
-        <v>24</v>
-      </c>
-      <c r="K65" t="s">
-        <v>20</v>
-      </c>
       <c r="L65" t="b">
         <v>1</v>
       </c>
@@ -3371,18 +3808,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B66" s="1">
         <v>45348</v>
       </c>
       <c r="C66" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="D66" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E66">
         <v>32</v>
@@ -3391,77 +3828,86 @@
         <v>32</v>
       </c>
       <c r="G66">
-        <v>2.7</v>
+        <v>8</v>
       </c>
       <c r="H66">
-        <v>8.1</v>
+        <v>24</v>
       </c>
       <c r="K66" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L66" t="b">
+        <v>1</v>
+      </c>
+      <c r="M66" t="b">
+        <v>1</v>
+      </c>
+      <c r="P66">
+        <v>81.2</v>
+      </c>
+      <c r="R66">
+        <v>45.1</v>
+      </c>
+      <c r="S66">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B67" s="1">
+        <v>45348</v>
+      </c>
+      <c r="C67" t="s">
+        <v>47</v>
+      </c>
+      <c r="D67" t="s">
+        <v>82</v>
+      </c>
+      <c r="E67">
+        <v>32</v>
+      </c>
+      <c r="F67">
+        <v>32</v>
+      </c>
+      <c r="G67">
+        <v>2.7</v>
+      </c>
+      <c r="H67">
+        <v>8.1</v>
+      </c>
+      <c r="K67" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B67" s="1"/>
-      <c r="J67">
+      <c r="B68" s="1"/>
+      <c r="J68">
         <v>4000</v>
       </c>
-      <c r="L67" t="b">
-        <v>1</v>
-      </c>
-      <c r="M67" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B68" s="1">
+      <c r="L68" t="b">
+        <v>1</v>
+      </c>
+      <c r="M68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B69" s="1">
         <v>45104</v>
-      </c>
-      <c r="C68" t="s">
-        <v>22</v>
-      </c>
-      <c r="D68" t="s">
-        <v>86</v>
-      </c>
-      <c r="E68">
-        <v>8.1920000000000002</v>
-      </c>
-      <c r="F68">
-        <v>8.1920000000000002</v>
-      </c>
-      <c r="G68">
-        <v>1.7</v>
-      </c>
-      <c r="H68">
-        <v>1.7</v>
-      </c>
-      <c r="K68" t="s">
-        <v>20</v>
-      </c>
-      <c r="L68" t="b">
-        <v>1</v>
-      </c>
-      <c r="M68" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B69" s="1">
-        <v>45398</v>
       </c>
       <c r="C69" t="s">
         <v>22</v>
       </c>
       <c r="D69" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E69">
         <v>8.1920000000000002</v>
@@ -3470,10 +3916,10 @@
         <v>8.1920000000000002</v>
       </c>
       <c r="G69">
-        <v>2.1</v>
+        <v>1.7</v>
       </c>
       <c r="H69">
-        <v>4.2</v>
+        <v>1.7</v>
       </c>
       <c r="K69" t="s">
         <v>20</v>
@@ -3485,147 +3931,191 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="B70" s="1">
-        <v>45246</v>
+        <v>45398</v>
       </c>
       <c r="C70" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="D70" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E70">
-        <v>32</v>
+        <v>8.1920000000000002</v>
       </c>
       <c r="F70">
-        <v>32</v>
+        <v>8.1920000000000002</v>
       </c>
       <c r="G70">
-        <v>3.4</v>
+        <v>2.1</v>
       </c>
       <c r="H70">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="K70" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L70" t="b">
+        <v>1</v>
+      </c>
+      <c r="M70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B71" s="1">
         <v>45246</v>
       </c>
       <c r="C71" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D71" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E71">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F71">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G71">
-        <v>1.7</v>
+        <v>3.4</v>
       </c>
       <c r="H71">
-        <v>1.7</v>
+        <v>3.4</v>
       </c>
       <c r="K71" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B72" s="1">
         <v>45246</v>
       </c>
       <c r="C72" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D72" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E72">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="F72">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="G72">
-        <v>8.5</v>
+        <v>1.7</v>
       </c>
       <c r="H72">
-        <v>8.5</v>
+        <v>1.7</v>
       </c>
       <c r="K72" t="s">
         <v>20</v>
       </c>
-      <c r="L72" t="b">
-        <v>1</v>
-      </c>
-      <c r="M72" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B73" s="1">
+        <v>45246</v>
+      </c>
+      <c r="C73" t="s">
+        <v>52</v>
+      </c>
+      <c r="D73" t="s">
+        <v>86</v>
+      </c>
+      <c r="E73">
+        <v>128</v>
+      </c>
+      <c r="F73">
+        <v>128</v>
+      </c>
+      <c r="G73">
+        <v>8.5</v>
+      </c>
+      <c r="H73">
+        <v>8.5</v>
+      </c>
+      <c r="K73" t="s">
+        <v>20</v>
+      </c>
+      <c r="L73" t="b">
+        <v>1</v>
+      </c>
+      <c r="M73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B74" s="1">
         <v>45234</v>
       </c>
-      <c r="L73" t="b">
-        <v>1</v>
-      </c>
-      <c r="M73" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B74" s="1">
+      <c r="L74" t="b">
+        <v>1</v>
+      </c>
+      <c r="M74" t="b">
+        <v>1</v>
+      </c>
+      <c r="P74">
+        <v>73</v>
+      </c>
+      <c r="R74">
+        <v>63.2</v>
+      </c>
+      <c r="S74">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B75" s="1">
         <v>44986</v>
       </c>
-      <c r="C74" t="s">
-        <v>31</v>
-      </c>
-      <c r="D74">
+      <c r="C75" t="s">
+        <v>29</v>
+      </c>
+      <c r="D75">
         <v>1085</v>
       </c>
-      <c r="J74">
+      <c r="J75">
         <v>329</v>
       </c>
-      <c r="K74" t="s">
+      <c r="K75" t="s">
         <v>20</v>
       </c>
-      <c r="L74" t="b">
-        <v>1</v>
-      </c>
-      <c r="M74" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B75" s="1"/>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L75" t="b">
+        <v>1</v>
+      </c>
+      <c r="M75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="1"/>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B77" s="1"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
fix(llm): appearance & minor bugs
</commit_message>
<xml_diff>
--- a/BogoInsight/crawlers/llm_additional_data.xlsx
+++ b/BogoInsight/crawlers/llm_additional_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ai\BogoInsight\BogoInsight\crawlers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80C0B05-102E-40B3-AA3E-44D8DC7DFE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EABF29-0186-4679-BB1D-8DDCEA8AFDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0BF4306-33E7-4D31-A9A6-85483F972F05}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="120">
   <si>
     <t>name</t>
   </si>
@@ -406,6 +406,14 @@
   </si>
   <si>
     <t>GPT-3.5 Turbo 0301</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>40*</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>300*</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1400,10 +1408,10 @@
   <dimension ref="A1:U90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R56" sqref="R56"/>
+      <selection pane="bottomRight" activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2975,7 +2983,7 @@
         <v>45355</v>
       </c>
       <c r="D43" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E43">
         <v>200</v>
@@ -3022,7 +3030,7 @@
         <v>45355</v>
       </c>
       <c r="D44" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="E44">
         <v>200</v>
@@ -3863,7 +3871,7 @@
         <v>47</v>
       </c>
       <c r="D67" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="E67">
         <v>32</v>

</xml_diff>

<commit_message>
feat(data): llm qwen update
</commit_message>
<xml_diff>
--- a/BogoInsight/crawlers/llm_additional_data.xlsx
+++ b/BogoInsight/crawlers/llm_additional_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ai\BogoInsight\BogoInsight\crawlers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EABF29-0186-4679-BB1D-8DDCEA8AFDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B256266-6AE1-4A60-BC18-BF714621929A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0BF4306-33E7-4D31-A9A6-85483F972F05}"/>
   </bookViews>
@@ -16,11 +16,12 @@
     <sheet name="20240508" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="122">
   <si>
     <t>name</t>
   </si>
@@ -414,6 +415,14 @@
   </si>
   <si>
     <t>300*</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qwen Long</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qwen VL</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1405,13 +1414,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFF9F69-317C-4CBC-86A8-E43FD4E7E879}">
-  <dimension ref="A1:U90"/>
+  <dimension ref="A1:U92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D72" sqref="D72"/>
+      <selection pane="bottomRight" activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3323,10 +3332,10 @@
         <v>2</v>
       </c>
       <c r="G51">
-        <v>0.85</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H51">
-        <v>0.85</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="K51" t="s">
         <v>43</v>
@@ -3361,10 +3370,10 @@
         <v>2</v>
       </c>
       <c r="G52">
-        <v>1.1000000000000001</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H52">
-        <v>1.1000000000000001</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="K52" t="s">
         <v>43</v>
@@ -3399,10 +3408,10 @@
         <v>2</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>0.49</v>
       </c>
       <c r="H53">
-        <v>0</v>
+        <v>0.98</v>
       </c>
       <c r="K53" t="s">
         <v>43</v>
@@ -3437,10 +3446,10 @@
         <v>2</v>
       </c>
       <c r="G54">
-        <v>2.8</v>
+        <v>0.7</v>
       </c>
       <c r="H54">
-        <v>2.8</v>
+        <v>1.4</v>
       </c>
       <c r="K54" t="s">
         <v>43</v>
@@ -3478,10 +3487,10 @@
         <v>2</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>0.98</v>
       </c>
       <c r="H55">
-        <v>0</v>
+        <v>1.96</v>
       </c>
       <c r="K55" t="s">
         <v>43</v>
@@ -3519,10 +3528,10 @@
         <v>2</v>
       </c>
       <c r="G56">
-        <v>1.1000000000000001</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H56">
-        <v>1.1000000000000001</v>
+        <v>0.84</v>
       </c>
       <c r="K56" t="s">
         <v>20</v>
@@ -3548,10 +3557,10 @@
         <v>2</v>
       </c>
       <c r="G57">
-        <v>2.8</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H57">
-        <v>2.8</v>
+        <v>1.68</v>
       </c>
       <c r="K57" t="s">
         <v>20</v>
@@ -3583,10 +3592,10 @@
         <v>2</v>
       </c>
       <c r="G58">
-        <v>16.600000000000001</v>
+        <v>16.8</v>
       </c>
       <c r="H58">
-        <v>16.600000000000001</v>
+        <v>16.8</v>
       </c>
       <c r="K58" t="s">
         <v>20</v>
@@ -3615,10 +3624,10 @@
         <v>2</v>
       </c>
       <c r="G59">
-        <v>16.600000000000001</v>
+        <v>5.6</v>
       </c>
       <c r="H59">
-        <v>16.600000000000001</v>
+        <v>16.8</v>
       </c>
       <c r="K59" t="s">
         <v>20</v>
@@ -3644,10 +3653,10 @@
         <v>2</v>
       </c>
       <c r="G60">
-        <v>16.600000000000001</v>
+        <v>5.6</v>
       </c>
       <c r="H60">
-        <v>16.600000000000001</v>
+        <v>16.8</v>
       </c>
       <c r="K60" t="s">
         <v>20</v>
@@ -3676,10 +3685,10 @@
         <v>2</v>
       </c>
       <c r="G61">
-        <v>16.600000000000001</v>
+        <v>5.6</v>
       </c>
       <c r="H61">
-        <v>16.600000000000001</v>
+        <v>16.8</v>
       </c>
       <c r="K61" t="s">
         <v>20</v>
@@ -3693,10 +3702,10 @@
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="B62" s="1">
-        <v>45261</v>
+        <v>45433</v>
       </c>
       <c r="C62" t="s">
         <v>42</v>
@@ -3705,36 +3714,39 @@
         <v>101</v>
       </c>
       <c r="E62">
-        <v>6</v>
+        <v>10000</v>
       </c>
       <c r="F62">
         <v>2</v>
       </c>
       <c r="G62">
-        <v>1.1000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H62">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I62">
-        <v>1.4</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="K62" t="s">
         <v>20</v>
       </c>
+      <c r="L62" t="b">
+        <v>1</v>
+      </c>
+      <c r="M62" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="B63" s="1">
-        <v>45261</v>
+        <v>45217</v>
       </c>
       <c r="C63" t="s">
         <v>42</v>
       </c>
-      <c r="D63" t="s">
-        <v>101</v>
+      <c r="D63">
+        <v>7</v>
       </c>
       <c r="E63">
         <v>6</v>
@@ -3743,229 +3755,235 @@
         <v>2</v>
       </c>
       <c r="G63">
-        <v>2.8</v>
+        <v>0</v>
       </c>
       <c r="H63">
-        <v>2.8</v>
+        <v>0</v>
       </c>
       <c r="I63">
-        <v>3.6</v>
+        <v>0</v>
       </c>
       <c r="K63" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="L63" t="b">
         <v>1</v>
       </c>
-      <c r="M63" t="b">
-        <v>1</v>
-      </c>
       <c r="N63" t="b">
         <v>1</v>
+      </c>
+      <c r="P63">
+        <v>58.2</v>
+      </c>
+      <c r="R63">
+        <v>31.6</v>
+      </c>
+      <c r="S63">
+        <v>11.6</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="B64" s="1">
-        <v>45196</v>
+        <v>45261</v>
+      </c>
+      <c r="C64" t="s">
+        <v>42</v>
+      </c>
+      <c r="D64" t="s">
+        <v>101</v>
       </c>
       <c r="E64">
-        <v>32.768000000000001</v>
+        <v>6</v>
       </c>
       <c r="F64">
-        <v>32.768000000000001</v>
+        <v>2</v>
       </c>
       <c r="G64">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H64">
-        <v>0</v>
-      </c>
-      <c r="L64" t="b">
-        <v>1</v>
-      </c>
-      <c r="M64" t="b">
-        <v>1</v>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I64">
+        <v>1.4</v>
+      </c>
+      <c r="K64" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="B65" s="1">
-        <v>45271</v>
+        <v>45261</v>
+      </c>
+      <c r="C65" t="s">
+        <v>42</v>
+      </c>
+      <c r="D65" t="s">
+        <v>101</v>
       </c>
       <c r="E65">
-        <v>32.768000000000001</v>
+        <v>6</v>
       </c>
       <c r="F65">
-        <v>32.768000000000001</v>
+        <v>2</v>
       </c>
       <c r="G65">
-        <v>0.24</v>
+        <v>2.8</v>
       </c>
       <c r="H65">
-        <v>0.24</v>
-      </c>
-      <c r="L65" t="b">
-        <v>1</v>
+        <v>2.8</v>
+      </c>
+      <c r="I65">
+        <v>3.6</v>
+      </c>
+      <c r="K65" t="s">
+        <v>20</v>
       </c>
       <c r="M65" t="b">
+        <v>1</v>
+      </c>
+      <c r="N65" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B66" s="1">
-        <v>45348</v>
-      </c>
-      <c r="C66" t="s">
-        <v>81</v>
-      </c>
-      <c r="D66" t="s">
-        <v>82</v>
+        <v>45196</v>
       </c>
       <c r="E66">
-        <v>32</v>
+        <v>32.768000000000001</v>
       </c>
       <c r="F66">
-        <v>32</v>
+        <v>32.768000000000001</v>
       </c>
       <c r="G66">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H66">
-        <v>24</v>
-      </c>
-      <c r="K66" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="L66" t="b">
         <v>1</v>
       </c>
       <c r="M66" t="b">
         <v>1</v>
-      </c>
-      <c r="P66">
-        <v>81.2</v>
-      </c>
-      <c r="R66">
-        <v>45.1</v>
-      </c>
-      <c r="S66">
-        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B67" s="1">
-        <v>45348</v>
-      </c>
-      <c r="C67" t="s">
-        <v>47</v>
-      </c>
-      <c r="D67" t="s">
-        <v>119</v>
+        <v>45271</v>
       </c>
       <c r="E67">
-        <v>32</v>
+        <v>32.768000000000001</v>
       </c>
       <c r="F67">
-        <v>32</v>
+        <v>32.768000000000001</v>
       </c>
       <c r="G67">
-        <v>2.7</v>
+        <v>0.24</v>
       </c>
       <c r="H67">
-        <v>8.1</v>
-      </c>
-      <c r="K67" t="s">
-        <v>20</v>
+        <v>0.24</v>
+      </c>
+      <c r="L67" t="b">
+        <v>1</v>
+      </c>
+      <c r="M67" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B68" s="1"/>
-      <c r="J68">
-        <v>4000</v>
+        <v>68</v>
+      </c>
+      <c r="B68" s="1">
+        <v>45348</v>
+      </c>
+      <c r="C68" t="s">
+        <v>81</v>
+      </c>
+      <c r="D68" t="s">
+        <v>82</v>
+      </c>
+      <c r="E68">
+        <v>32</v>
+      </c>
+      <c r="F68">
+        <v>32</v>
+      </c>
+      <c r="G68">
+        <v>8</v>
+      </c>
+      <c r="H68">
+        <v>24</v>
+      </c>
+      <c r="K68" t="s">
+        <v>20</v>
       </c>
       <c r="L68" t="b">
         <v>1</v>
       </c>
       <c r="M68" t="b">
         <v>1</v>
+      </c>
+      <c r="P68">
+        <v>81.2</v>
+      </c>
+      <c r="R68">
+        <v>45.1</v>
+      </c>
+      <c r="S68">
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="B69" s="1">
-        <v>45104</v>
+        <v>45348</v>
       </c>
       <c r="C69" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="D69" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="E69">
-        <v>8.1920000000000002</v>
+        <v>32</v>
       </c>
       <c r="F69">
-        <v>8.1920000000000002</v>
+        <v>32</v>
       </c>
       <c r="G69">
-        <v>1.7</v>
+        <v>2.7</v>
       </c>
       <c r="H69">
-        <v>1.7</v>
+        <v>8.1</v>
       </c>
       <c r="K69" t="s">
         <v>20</v>
       </c>
-      <c r="L69" t="b">
-        <v>1</v>
-      </c>
-      <c r="M69" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B70" s="1">
-        <v>45398</v>
-      </c>
-      <c r="C70" t="s">
-        <v>22</v>
-      </c>
-      <c r="D70" t="s">
-        <v>85</v>
-      </c>
-      <c r="E70">
-        <v>8.1920000000000002</v>
-      </c>
-      <c r="F70">
-        <v>8.1920000000000002</v>
-      </c>
-      <c r="G70">
-        <v>2.1</v>
-      </c>
-      <c r="H70">
-        <v>4.2</v>
-      </c>
-      <c r="K70" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="B70" s="1"/>
+      <c r="J70">
+        <v>4000</v>
       </c>
       <c r="L70" t="b">
         <v>1</v>
@@ -3976,65 +3994,77 @@
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B71" s="1">
-        <v>45246</v>
+        <v>45104</v>
       </c>
       <c r="C71" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="D71" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E71">
-        <v>32</v>
+        <v>8.1920000000000002</v>
       </c>
       <c r="F71">
-        <v>32</v>
+        <v>8.1920000000000002</v>
       </c>
       <c r="G71">
-        <v>3.4</v>
+        <v>1.7</v>
       </c>
       <c r="H71">
-        <v>3.4</v>
+        <v>1.7</v>
       </c>
       <c r="K71" t="s">
         <v>20</v>
       </c>
+      <c r="L71" t="b">
+        <v>1</v>
+      </c>
+      <c r="M71" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="B72" s="1">
-        <v>45246</v>
+        <v>45398</v>
       </c>
       <c r="C72" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="D72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E72">
-        <v>8</v>
+        <v>8.1920000000000002</v>
       </c>
       <c r="F72">
-        <v>8</v>
+        <v>8.1920000000000002</v>
       </c>
       <c r="G72">
-        <v>1.7</v>
+        <v>2.1</v>
       </c>
       <c r="H72">
-        <v>1.7</v>
+        <v>4.2</v>
       </c>
       <c r="K72" t="s">
         <v>20</v>
       </c>
+      <c r="L72" t="b">
+        <v>1</v>
+      </c>
+      <c r="M72" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B73" s="1">
         <v>45246</v>
@@ -4046,65 +4076,74 @@
         <v>86</v>
       </c>
       <c r="E73">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="F73">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="G73">
-        <v>8.5</v>
+        <v>3.4</v>
       </c>
       <c r="H73">
-        <v>8.5</v>
+        <v>3.4</v>
       </c>
       <c r="K73" t="s">
         <v>20</v>
       </c>
-      <c r="L73" t="b">
-        <v>1</v>
-      </c>
-      <c r="M73" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B74" s="1">
-        <v>45234</v>
-      </c>
-      <c r="L74" t="b">
-        <v>1</v>
-      </c>
-      <c r="M74" t="b">
-        <v>1</v>
-      </c>
-      <c r="P74">
-        <v>73</v>
-      </c>
-      <c r="R74">
-        <v>63.2</v>
-      </c>
-      <c r="S74">
-        <v>23.9</v>
+        <v>45246</v>
+      </c>
+      <c r="C74" t="s">
+        <v>52</v>
+      </c>
+      <c r="D74" t="s">
+        <v>86</v>
+      </c>
+      <c r="E74">
+        <v>8</v>
+      </c>
+      <c r="F74">
+        <v>8</v>
+      </c>
+      <c r="G74">
+        <v>1.7</v>
+      </c>
+      <c r="H74">
+        <v>1.7</v>
+      </c>
+      <c r="K74" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="B75" s="1">
-        <v>44986</v>
+        <v>45246</v>
       </c>
       <c r="C75" t="s">
-        <v>29</v>
-      </c>
-      <c r="D75">
-        <v>1085</v>
-      </c>
-      <c r="J75">
-        <v>329</v>
+        <v>52</v>
+      </c>
+      <c r="D75" t="s">
+        <v>86</v>
+      </c>
+      <c r="E75">
+        <v>128</v>
+      </c>
+      <c r="F75">
+        <v>128</v>
+      </c>
+      <c r="G75">
+        <v>8.5</v>
+      </c>
+      <c r="H75">
+        <v>8.5</v>
       </c>
       <c r="K75" t="s">
         <v>20</v>
@@ -4117,13 +4156,62 @@
       </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B76" s="1"/>
+      <c r="A76" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B76" s="1">
+        <v>45234</v>
+      </c>
+      <c r="L76" t="b">
+        <v>1</v>
+      </c>
+      <c r="M76" t="b">
+        <v>1</v>
+      </c>
+      <c r="P76">
+        <v>73</v>
+      </c>
+      <c r="R76">
+        <v>63.2</v>
+      </c>
+      <c r="S76">
+        <v>23.9</v>
+      </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B77" s="1"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="1"/>
+      <c r="A77" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" s="1">
+        <v>44986</v>
+      </c>
+      <c r="C77" t="s">
+        <v>29</v>
+      </c>
+      <c r="D77">
+        <v>1085</v>
+      </c>
+      <c r="J77">
+        <v>329</v>
+      </c>
+      <c r="K77" t="s">
+        <v>20</v>
+      </c>
+      <c r="L77" t="b">
+        <v>1</v>
+      </c>
+      <c r="M77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
feat(llm): add 01.AI & Zhipu AI models
</commit_message>
<xml_diff>
--- a/BogoInsight/crawlers/llm_additional_data.xlsx
+++ b/BogoInsight/crawlers/llm_additional_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ai\BogoInsight\BogoInsight\crawlers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B256266-6AE1-4A60-BC18-BF714621929A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB37A26F-8E1B-4597-8787-8CACB321DEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0BF4306-33E7-4D31-A9A6-85483F972F05}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="130">
   <si>
     <t>name</t>
   </si>
@@ -423,6 +423,38 @@
   </si>
   <si>
     <t>Qwen VL</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yi Large</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>01.AI</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>100*</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yi Medium</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>10*</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GLM-4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhipu AI</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GLM-4V</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1417,10 +1449,10 @@
   <dimension ref="A1:U92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H56" sqref="H56"/>
+      <selection pane="bottomRight" activeCell="I84" sqref="I84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4205,12 +4237,173 @@
       </c>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B78" s="1"/>
+      <c r="A78" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B78" s="1">
+        <v>45425</v>
+      </c>
+      <c r="C78" t="s">
+        <v>123</v>
+      </c>
+      <c r="D78" t="s">
+        <v>124</v>
+      </c>
+      <c r="E78">
+        <v>16</v>
+      </c>
+      <c r="F78">
+        <v>16</v>
+      </c>
+      <c r="G78">
+        <v>2.8</v>
+      </c>
+      <c r="H78">
+        <v>2.8</v>
+      </c>
+      <c r="K78" t="s">
+        <v>20</v>
+      </c>
+      <c r="L78" t="b">
+        <v>1</v>
+      </c>
+      <c r="M78" t="b">
+        <v>1</v>
+      </c>
+      <c r="P78">
+        <v>83.8</v>
+      </c>
+      <c r="R78">
+        <v>82.3</v>
+      </c>
+      <c r="S78">
+        <v>62.4</v>
+      </c>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B79" s="1"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B79" s="1">
+        <v>45425</v>
+      </c>
+      <c r="C79" t="s">
+        <v>123</v>
+      </c>
+      <c r="D79" t="s">
+        <v>126</v>
+      </c>
+      <c r="E79">
+        <v>16</v>
+      </c>
+      <c r="F79">
+        <v>16</v>
+      </c>
+      <c r="G79">
+        <v>0.35</v>
+      </c>
+      <c r="H79">
+        <v>0.35</v>
+      </c>
+      <c r="K79" t="s">
+        <v>20</v>
+      </c>
+      <c r="P79">
+        <v>76.8</v>
+      </c>
+      <c r="R79">
+        <v>75.2</v>
+      </c>
+      <c r="S79">
+        <v>50.1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B80" s="1">
+        <v>45307</v>
+      </c>
+      <c r="C80" t="s">
+        <v>128</v>
+      </c>
+      <c r="D80" t="s">
+        <v>83</v>
+      </c>
+      <c r="E80">
+        <v>128</v>
+      </c>
+      <c r="F80">
+        <v>8.1920000000000002</v>
+      </c>
+      <c r="G80">
+        <v>14.1</v>
+      </c>
+      <c r="H80">
+        <v>14.1</v>
+      </c>
+      <c r="K80" t="s">
+        <v>20</v>
+      </c>
+      <c r="L80" t="b">
+        <v>1</v>
+      </c>
+      <c r="M80" t="b">
+        <v>1</v>
+      </c>
+      <c r="P80">
+        <v>81.5</v>
+      </c>
+      <c r="R80">
+        <v>72</v>
+      </c>
+      <c r="S80">
+        <v>47.9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B81" s="1">
+        <v>45307</v>
+      </c>
+      <c r="C81" t="s">
+        <v>128</v>
+      </c>
+      <c r="D81" t="s">
+        <v>83</v>
+      </c>
+      <c r="E81">
+        <v>2</v>
+      </c>
+      <c r="F81">
+        <v>2</v>
+      </c>
+      <c r="G81">
+        <v>14.1</v>
+      </c>
+      <c r="H81">
+        <v>14.1</v>
+      </c>
+      <c r="I81">
+        <v>14.8</v>
+      </c>
+      <c r="K81" t="s">
+        <v>20</v>
+      </c>
+      <c r="L81" t="b">
+        <v>1</v>
+      </c>
+      <c r="M81" t="b">
+        <v>1</v>
+      </c>
+      <c r="N81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B92" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(llm): latest model update
</commit_message>
<xml_diff>
--- a/BogoInsight/crawlers/llm_additional_data.xlsx
+++ b/BogoInsight/crawlers/llm_additional_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ai\BogoInsight\BogoInsight\crawlers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E30A77-4147-425F-83F3-6963B02107C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929AFEC1-B875-479D-82D2-78DE9A3F1051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0BF4306-33E7-4D31-A9A6-85483F972F05}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="147">
   <si>
     <t>name</t>
   </si>
@@ -136,332 +136,394 @@
     <t>Claude 2</t>
   </si>
   <si>
+    <t>Llama 2 license</t>
+  </si>
+  <si>
+    <t>Llama 2 13B</t>
+  </si>
+  <si>
+    <t>Qwen 7B</t>
+  </si>
+  <si>
+    <t>Aliyun</t>
+  </si>
+  <si>
+    <t>tongyi-qianwen</t>
+  </si>
+  <si>
+    <t>Qwen 14B</t>
+  </si>
+  <si>
+    <t>Mistral 7B</t>
+  </si>
+  <si>
+    <t>Mistral AI</t>
+  </si>
+  <si>
+    <t>Grok-1</t>
+  </si>
+  <si>
+    <t>GPT-4 Turbo</t>
+  </si>
+  <si>
+    <t>GPT-3.5 Turbo 16K 1106</t>
+  </si>
+  <si>
+    <t>Moonshot V1 32K</t>
+  </si>
+  <si>
+    <t>Moonshot</t>
+  </si>
+  <si>
+    <t>Moonshot V1 8K</t>
+  </si>
+  <si>
+    <t>Moonshot V1 128K</t>
+  </si>
+  <si>
+    <t>Claude 2.1</t>
+  </si>
+  <si>
+    <t>Qwen 1.8B</t>
+  </si>
+  <si>
+    <t>Qwen 72B</t>
+  </si>
+  <si>
+    <t>Mixtral 8x7B</t>
+  </si>
+  <si>
+    <t>GPT-4 Turbo 0125</t>
+  </si>
+  <si>
+    <t>GPT-3.5 Turbo 16K 0125</t>
+  </si>
+  <si>
+    <t>Qwen1.5 72B</t>
+  </si>
+  <si>
+    <t>Qwen1.5 7B</t>
+  </si>
+  <si>
+    <t>Qwen1.5 32B</t>
+  </si>
+  <si>
+    <t>Qwen1.5 14B</t>
+  </si>
+  <si>
+    <t>Qwen1.5 1.8B</t>
+  </si>
+  <si>
+    <t>Qwen1.5 0.5B</t>
+  </si>
+  <si>
+    <t>Gemma</t>
+  </si>
+  <si>
+    <t>Mistral Large</t>
+  </si>
+  <si>
+    <t>Mistral Medium</t>
+  </si>
+  <si>
+    <t>Claude 3 Sonnet</t>
+  </si>
+  <si>
+    <t>Claude 3 Opus</t>
+  </si>
+  <si>
+    <t>Claude 3 Haiku</t>
+  </si>
+  <si>
+    <t>GPT-4 Turbo 2024-04-09</t>
+  </si>
+  <si>
+    <t>Ernie 4.0</t>
+  </si>
+  <si>
+    <t>Llama 3 8B</t>
+  </si>
+  <si>
+    <t>Llama 3 license</t>
+  </si>
+  <si>
+    <t>Llama 3 70B</t>
+  </si>
+  <si>
+    <t>Qwen1.5 110B</t>
+  </si>
+  <si>
+    <t>PanGu-Σ</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2000*</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mistral AI</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000*</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>130*</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>175*</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1750*</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>200*</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>has visual</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>has audio</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gemini 1.0 Pro</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Google</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gemini 1.5 Pro</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gemini 1.0 Ultra</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gemini 1.0 Nano</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gemini 1.5 Flash</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gemini 1.5 Pro 2024-05</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gemma 2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PaliGemma</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qwen Turbo</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qwen Plus</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qwen2 Max 1201</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>110*</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qwen2.5 Max 0428</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qwen2 Max 0403</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qwen2 Max 0107</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qwen VL Plus</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qwen VL Max</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>72*</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPT-4o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Llama 2 7B</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DROP</t>
+  </si>
+  <si>
+    <t>HumanEval</t>
+  </si>
+  <si>
+    <t>MATH</t>
+  </si>
+  <si>
+    <t>MMLU</t>
+  </si>
+  <si>
+    <t>MMMU</t>
+  </si>
+  <si>
+    <t>MathVista</t>
+  </si>
+  <si>
+    <t>GPT-3.5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPT-3.5 Turbo 0301</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>40*</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>300*</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qwen Long</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qwen VL</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yi Large</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>01.AI</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>100*</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yi Medium</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>10*</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GLM-4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhipu AI</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GLM-4V</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPT-4o-mini</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Claude 3.5 Sonnet</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phi-1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Microsoft</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIT</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phi-1.5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phi-2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phi-3 Mini</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phi-3 Small</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phi-3 Medium</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phi-3 Vision</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qwen2 0.5B</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qwen2 1.5B</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qwen2 7B</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qwen2 57B-A14B</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qwen2 72B</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPT-4 Vision Preview</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>Llama 2 70B</t>
-  </si>
-  <si>
-    <t>Llama 2 license</t>
-  </si>
-  <si>
-    <t>Llama 2 13B</t>
-  </si>
-  <si>
-    <t>Qwen 7B</t>
-  </si>
-  <si>
-    <t>Aliyun</t>
-  </si>
-  <si>
-    <t>tongyi-qianwen</t>
-  </si>
-  <si>
-    <t>Qwen 14B</t>
-  </si>
-  <si>
-    <t>GPT-4 Vision Preview</t>
-  </si>
-  <si>
-    <t>Mistral 7B</t>
-  </si>
-  <si>
-    <t>Mistral AI</t>
-  </si>
-  <si>
-    <t>Grok-1</t>
-  </si>
-  <si>
-    <t>GPT-4 Turbo</t>
-  </si>
-  <si>
-    <t>GPT-3.5 Turbo 16K 1106</t>
-  </si>
-  <si>
-    <t>Moonshot V1 32K</t>
-  </si>
-  <si>
-    <t>Moonshot</t>
-  </si>
-  <si>
-    <t>Moonshot V1 8K</t>
-  </si>
-  <si>
-    <t>Moonshot V1 128K</t>
-  </si>
-  <si>
-    <t>Claude 2.1</t>
-  </si>
-  <si>
-    <t>Qwen 1.8B</t>
-  </si>
-  <si>
-    <t>Qwen 72B</t>
-  </si>
-  <si>
-    <t>Mixtral 8x7B</t>
-  </si>
-  <si>
-    <t>GPT-4 Turbo 0125</t>
-  </si>
-  <si>
-    <t>GPT-3.5 Turbo 16K 0125</t>
-  </si>
-  <si>
-    <t>Qwen1.5 72B</t>
-  </si>
-  <si>
-    <t>Qwen1.5 7B</t>
-  </si>
-  <si>
-    <t>Qwen1.5 32B</t>
-  </si>
-  <si>
-    <t>Qwen1.5 14B</t>
-  </si>
-  <si>
-    <t>Qwen1.5 1.8B</t>
-  </si>
-  <si>
-    <t>Qwen1.5 0.5B</t>
-  </si>
-  <si>
-    <t>Gemma</t>
-  </si>
-  <si>
-    <t>Mistral Large</t>
-  </si>
-  <si>
-    <t>Mistral Medium</t>
-  </si>
-  <si>
-    <t>Claude 3 Sonnet</t>
-  </si>
-  <si>
-    <t>Claude 3 Opus</t>
-  </si>
-  <si>
-    <t>Claude 3 Haiku</t>
-  </si>
-  <si>
-    <t>GPT-4 Turbo 2024-04-09</t>
-  </si>
-  <si>
-    <t>Ernie 4.0</t>
-  </si>
-  <si>
-    <t>Llama 3 8B</t>
-  </si>
-  <si>
-    <t>Llama 3 license</t>
-  </si>
-  <si>
-    <t>Llama 3 70B</t>
-  </si>
-  <si>
-    <t>Qwen1.5 110B</t>
-  </si>
-  <si>
-    <t>PanGu-Σ</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>2000*</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mistral AI</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1000*</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>130*</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>175*</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1750*</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>200*</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>has visual</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>has audio</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gemini 1.0 Pro</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Google</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gemini 1.5 Pro</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gemini 1.0 Ultra</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gemini 1.0 Nano</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gemini 1.5 Flash</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gemini 1.5 Pro 2024-05</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gemma 2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>PaliGemma</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qwen Turbo</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qwen Plus</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qwen2 Max 1201</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>110*</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qwen2.5 Max 0428</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qwen2 Max 0403</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qwen2 Max 0107</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qwen VL Plus</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qwen VL Max</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>72*</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>GPT-4o</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Llama 2 7B</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>DROP</t>
-  </si>
-  <si>
-    <t>HumanEval</t>
-  </si>
-  <si>
-    <t>MATH</t>
-  </si>
-  <si>
-    <t>MMLU</t>
-  </si>
-  <si>
-    <t>MMMU</t>
-  </si>
-  <si>
-    <t>MathVista</t>
-  </si>
-  <si>
-    <t>GPT-3.5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>GPT-3.5 Turbo 0301</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>40*</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>300*</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qwen Long</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qwen VL</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yi Large</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>01.AI</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>100*</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yi Medium</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>10*</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>GLM-4</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Zhipu AI</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>GLM-4V</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qwen1.5 1.5B</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qwen1.5 57B-A14B</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anthropic</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1453,13 +1515,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFF9F69-317C-4CBC-86A8-E43FD4E7E879}">
-  <dimension ref="A1:U91"/>
+  <dimension ref="A1:U95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K85" sqref="K85"/>
+      <selection pane="bottomRight" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1523,28 +1585,28 @@
         <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="P1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -1591,7 +1653,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B5" s="1">
         <v>44893</v>
@@ -1623,7 +1685,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B6" s="1">
         <v>44986</v>
@@ -1696,7 +1758,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1">
         <v>45236</v>
@@ -1725,7 +1787,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B9" s="1">
         <v>45316</v>
@@ -1888,7 +1950,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>45</v>
+        <v>144</v>
       </c>
       <c r="B14" s="1">
         <v>45194</v>
@@ -1926,7 +1988,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B15" s="1">
         <v>45236</v>
@@ -1967,7 +2029,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" s="1">
         <v>45316</v>
@@ -1996,7 +2058,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B17" s="1">
         <v>45391</v>
@@ -2040,7 +2102,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B18" s="1">
         <v>45425</v>
@@ -2049,7 +2111,7 @@
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E18">
         <v>128</v>
@@ -2064,7 +2126,7 @@
         <v>15</v>
       </c>
       <c r="I18">
-        <v>2.3119999999999998</v>
+        <v>7.2249999999999996</v>
       </c>
       <c r="K18" t="s">
         <v>20</v>
@@ -2099,26 +2161,64 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="J19">
-        <v>5.4</v>
-      </c>
-      <c r="L19" t="b">
-        <v>1</v>
-      </c>
-      <c r="M19" t="b">
-        <v>1</v>
+        <v>128</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45491</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19">
+        <v>128</v>
+      </c>
+      <c r="F19">
+        <v>16.384</v>
+      </c>
+      <c r="G19">
+        <v>0.15</v>
+      </c>
+      <c r="H19">
+        <v>0.6</v>
+      </c>
+      <c r="I19">
+        <v>7.2249999999999996</v>
+      </c>
+      <c r="K19" t="s">
+        <v>20</v>
+      </c>
+      <c r="N19" t="b">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>82</v>
+      </c>
+      <c r="Q19">
+        <v>79.7</v>
+      </c>
+      <c r="R19">
+        <v>87.2</v>
+      </c>
+      <c r="S19">
+        <v>70.2</v>
+      </c>
+      <c r="T19">
+        <v>59.4</v>
+      </c>
+      <c r="U19">
+        <v>56.7</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1"/>
       <c r="J20">
-        <v>34</v>
+        <v>5.4</v>
       </c>
       <c r="L20" t="b">
         <v>1</v>
@@ -2129,11 +2229,11 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1"/>
       <c r="J21">
-        <v>1400</v>
+        <v>34</v>
       </c>
       <c r="L21" t="b">
         <v>1</v>
@@ -2144,11 +2244,11 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1"/>
       <c r="J22">
-        <v>768</v>
+        <v>1400</v>
       </c>
       <c r="L22" t="b">
         <v>1</v>
@@ -2159,25 +2259,11 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="1">
-        <v>45056</v>
-      </c>
-      <c r="E23">
-        <v>25.803999999999998</v>
-      </c>
-      <c r="F23">
-        <v>2.9670000000000001</v>
-      </c>
-      <c r="G23">
-        <v>0.25</v>
-      </c>
-      <c r="H23">
-        <v>0.5</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B23" s="1"/>
       <c r="J23">
-        <v>3600</v>
+        <v>768</v>
       </c>
       <c r="L23" t="b">
         <v>1</v>
@@ -2188,51 +2274,39 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="B24" s="1">
-        <v>45343</v>
+        <v>45056</v>
       </c>
       <c r="E24">
-        <v>8.1920000000000002</v>
+        <v>25.803999999999998</v>
       </c>
       <c r="F24">
-        <v>8.1920000000000002</v>
+        <v>2.9670000000000001</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J24">
-        <v>6000</v>
+        <v>3600</v>
       </c>
       <c r="L24" t="b">
         <v>1</v>
       </c>
-      <c r="P24">
-        <v>64.3</v>
-      </c>
-      <c r="R24">
-        <v>32.299999999999997</v>
-      </c>
-      <c r="S24">
-        <v>24.3</v>
+      <c r="M24" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="B25" s="1">
-        <v>45426</v>
-      </c>
-      <c r="C25" t="s">
-        <v>90</v>
-      </c>
-      <c r="D25">
-        <v>27</v>
+        <v>45343</v>
       </c>
       <c r="E25">
         <v>8.1920000000000002</v>
@@ -2246,28 +2320,34 @@
       <c r="H25">
         <v>0</v>
       </c>
-      <c r="K25" t="s">
-        <v>16</v>
-      </c>
-      <c r="M25" t="b">
+      <c r="J25">
+        <v>6000</v>
+      </c>
+      <c r="L25" t="b">
         <v>1</v>
       </c>
       <c r="P25">
-        <v>75</v>
+        <v>64.3</v>
+      </c>
+      <c r="R25">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="S25">
+        <v>24.3</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B26" s="1">
         <v>45426</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E26">
         <v>8.1920000000000002</v>
@@ -2281,96 +2361,69 @@
       <c r="H26">
         <v>0</v>
       </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
       <c r="K26" t="s">
         <v>16</v>
       </c>
-      <c r="L26" t="b">
-        <v>1</v>
-      </c>
       <c r="M26" t="b">
         <v>1</v>
       </c>
-      <c r="N26" t="b">
-        <v>1</v>
+      <c r="P26">
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B27" s="1">
-        <v>45283</v>
+        <v>45426</v>
       </c>
       <c r="C27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D27">
-        <v>1600</v>
+        <v>3</v>
       </c>
       <c r="E27">
-        <v>91.727999999999994</v>
+        <v>8.1920000000000002</v>
       </c>
       <c r="F27">
-        <v>22.937000000000001</v>
+        <v>8.1920000000000002</v>
       </c>
       <c r="G27">
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="H27">
-        <v>0.375</v>
+        <v>0</v>
       </c>
       <c r="I27">
-        <v>2.5</v>
-      </c>
-      <c r="J27">
-        <v>1560</v>
+        <v>0</v>
       </c>
       <c r="K27" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L27" t="b">
         <v>1</v>
       </c>
+      <c r="M27" t="b">
+        <v>1</v>
+      </c>
       <c r="N27" t="b">
         <v>1</v>
-      </c>
-      <c r="O27" t="b">
-        <v>1</v>
-      </c>
-      <c r="P27">
-        <v>71.8</v>
-      </c>
-      <c r="Q27">
-        <v>74.099999999999994</v>
-      </c>
-      <c r="R27">
-        <v>67.7</v>
-      </c>
-      <c r="S27">
-        <v>32.6</v>
-      </c>
-      <c r="T27">
-        <v>47.9</v>
-      </c>
-      <c r="U27">
-        <v>46.6</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B28" s="1">
         <v>45283</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D28">
-        <v>100</v>
+        <v>1600</v>
       </c>
       <c r="E28">
         <v>91.727999999999994</v>
@@ -2378,9 +2431,24 @@
       <c r="F28">
         <v>22.937000000000001</v>
       </c>
+      <c r="G28">
+        <v>0.125</v>
+      </c>
+      <c r="H28">
+        <v>0.375</v>
+      </c>
+      <c r="I28">
+        <v>2.5</v>
+      </c>
+      <c r="J28">
+        <v>1560</v>
+      </c>
       <c r="K28" t="s">
         <v>20</v>
       </c>
+      <c r="L28" t="b">
+        <v>1</v>
+      </c>
       <c r="N28" t="b">
         <v>1</v>
       </c>
@@ -2388,30 +2456,36 @@
         <v>1</v>
       </c>
       <c r="P28">
-        <v>58.8</v>
+        <v>71.8</v>
+      </c>
+      <c r="Q28">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="R28">
+        <v>67.7</v>
       </c>
       <c r="S28">
-        <v>22.8</v>
+        <v>32.6</v>
       </c>
       <c r="T28">
-        <v>32.6</v>
+        <v>47.9</v>
       </c>
       <c r="U28">
-        <v>30.6</v>
+        <v>46.6</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B29" s="1">
-        <v>45330</v>
+        <v>45283</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
-      </c>
-      <c r="D29" t="s">
-        <v>80</v>
+        <v>88</v>
+      </c>
+      <c r="D29">
+        <v>100</v>
       </c>
       <c r="E29">
         <v>91.727999999999994</v>
@@ -2422,9 +2496,6 @@
       <c r="K29" t="s">
         <v>20</v>
       </c>
-      <c r="M29" t="b">
-        <v>1</v>
-      </c>
       <c r="N29" t="b">
         <v>1</v>
       </c>
@@ -2432,56 +2503,41 @@
         <v>1</v>
       </c>
       <c r="P29">
-        <v>83.7</v>
-      </c>
-      <c r="Q29">
-        <v>82.4</v>
-      </c>
-      <c r="R29">
-        <v>74.400000000000006</v>
+        <v>58.8</v>
       </c>
       <c r="S29">
-        <v>53.2</v>
+        <v>22.8</v>
       </c>
       <c r="T29">
-        <v>59.4</v>
+        <v>32.6</v>
       </c>
       <c r="U29">
-        <v>53</v>
+        <v>30.6</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B30" s="1">
-        <v>45337</v>
+        <v>45330</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E30">
-        <v>1000</v>
+        <v>91.727999999999994</v>
       </c>
       <c r="F30">
         <v>22.937000000000001</v>
       </c>
-      <c r="G30">
-        <v>2.5</v>
-      </c>
-      <c r="H30">
-        <v>7.5</v>
-      </c>
-      <c r="I30">
-        <v>2.65</v>
-      </c>
       <c r="K30" t="s">
         <v>20</v>
       </c>
-      <c r="L30" t="b">
+      <c r="M30" t="b">
         <v>1</v>
       </c>
       <c r="N30" t="b">
@@ -2491,39 +2547,39 @@
         <v>1</v>
       </c>
       <c r="P30">
-        <v>81.900000000000006</v>
+        <v>83.7</v>
       </c>
       <c r="Q30">
-        <v>83.5</v>
+        <v>82.4</v>
       </c>
       <c r="R30">
-        <v>84.1</v>
+        <v>74.400000000000006</v>
       </c>
       <c r="S30">
-        <v>58.5</v>
+        <v>53.2</v>
       </c>
       <c r="T30">
-        <v>58.5</v>
+        <v>59.4</v>
       </c>
       <c r="U30">
-        <v>54.7</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B31" s="1">
-        <v>45426</v>
+        <v>45337</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E31">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="F31">
         <v>22.937000000000001</v>
@@ -2540,7 +2596,7 @@
       <c r="K31" t="s">
         <v>20</v>
       </c>
-      <c r="M31" t="b">
+      <c r="L31" t="b">
         <v>1</v>
       </c>
       <c r="N31" t="b">
@@ -2550,55 +2606,58 @@
         <v>1</v>
       </c>
       <c r="P31">
-        <v>85.9</v>
+        <v>81.900000000000006</v>
       </c>
       <c r="Q31">
-        <v>74.900000000000006</v>
+        <v>83.5</v>
       </c>
       <c r="R31">
         <v>84.1</v>
       </c>
       <c r="S31">
-        <v>67.7</v>
+        <v>58.5</v>
       </c>
       <c r="T31">
-        <v>62.2</v>
+        <v>58.5</v>
       </c>
       <c r="U31">
-        <v>63.9</v>
+        <v>54.7</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B32" s="1">
         <v>45426</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D32" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E32">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="F32">
         <v>22.937000000000001</v>
       </c>
       <c r="G32">
-        <v>0.25</v>
+        <v>2.5</v>
       </c>
       <c r="H32">
-        <v>0.75</v>
+        <v>7.5</v>
       </c>
       <c r="I32">
-        <v>0.26500000000000001</v>
+        <v>2.65</v>
       </c>
       <c r="K32" t="s">
         <v>20</v>
       </c>
+      <c r="M32" t="b">
+        <v>1</v>
+      </c>
       <c r="N32" t="b">
         <v>1</v>
       </c>
@@ -2606,95 +2665,101 @@
         <v>1</v>
       </c>
       <c r="P32">
-        <v>78.900000000000006</v>
+        <v>85.9</v>
       </c>
       <c r="Q32">
-        <v>78.400000000000006</v>
+        <v>74.900000000000006</v>
       </c>
       <c r="R32">
-        <v>74.3</v>
+        <v>84.1</v>
       </c>
       <c r="S32">
-        <v>54.9</v>
+        <v>67.7</v>
       </c>
       <c r="T32">
-        <v>56.1</v>
+        <v>62.2</v>
       </c>
       <c r="U32">
-        <v>58.4</v>
+        <v>63.9</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="D33">
-        <v>65</v>
-      </c>
-      <c r="J33">
-        <v>1400</v>
-      </c>
-      <c r="L33" t="b">
-        <v>1</v>
-      </c>
-      <c r="M33" t="b">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="B33" s="1">
+        <v>45426</v>
+      </c>
+      <c r="C33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33">
+        <v>1000</v>
+      </c>
+      <c r="F33">
+        <v>22.937000000000001</v>
+      </c>
+      <c r="G33">
+        <v>0.25</v>
+      </c>
+      <c r="H33">
+        <v>0.75</v>
+      </c>
+      <c r="I33">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="K33" t="s">
+        <v>20</v>
+      </c>
+      <c r="N33" t="b">
+        <v>1</v>
+      </c>
+      <c r="O33" t="b">
+        <v>1</v>
+      </c>
+      <c r="P33">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="Q33">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="R33">
+        <v>74.3</v>
+      </c>
+      <c r="S33">
+        <v>54.9</v>
+      </c>
+      <c r="T33">
+        <v>56.1</v>
+      </c>
+      <c r="U33">
+        <v>58.4</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="1">
-        <v>45125</v>
-      </c>
-      <c r="C34" t="s">
-        <v>28</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B34" s="1"/>
       <c r="D34">
-        <v>70</v>
-      </c>
-      <c r="E34">
-        <v>4.0960000000000001</v>
-      </c>
-      <c r="F34">
-        <v>4.0960000000000001</v>
-      </c>
-      <c r="G34">
-        <v>0.64</v>
-      </c>
-      <c r="H34">
-        <v>0.8</v>
+        <v>65</v>
       </c>
       <c r="J34">
-        <v>2000</v>
-      </c>
-      <c r="K34" t="s">
-        <v>39</v>
+        <v>1400</v>
       </c>
       <c r="L34" t="b">
         <v>1</v>
       </c>
       <c r="M34" t="b">
         <v>1</v>
-      </c>
-      <c r="P34">
-        <v>69.7</v>
-      </c>
-      <c r="Q34">
-        <v>70.2</v>
-      </c>
-      <c r="R34">
-        <v>25.6</v>
-      </c>
-      <c r="S34">
-        <v>11.6</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>40</v>
+        <v>145</v>
       </c>
       <c r="B35" s="1">
         <v>45125</v>
@@ -2703,7 +2768,7 @@
         <v>28</v>
       </c>
       <c r="D35">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="E35">
         <v>4.0960000000000001</v>
@@ -2712,33 +2777,39 @@
         <v>4.0960000000000001</v>
       </c>
       <c r="G35">
-        <v>0.13</v>
+        <v>0.64</v>
       </c>
       <c r="H35">
-        <v>0.13</v>
+        <v>0.8</v>
       </c>
       <c r="J35">
         <v>2000</v>
       </c>
       <c r="K35" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="L35" t="b">
+        <v>1</v>
+      </c>
+      <c r="M35" t="b">
+        <v>1</v>
       </c>
       <c r="P35">
-        <v>53.8</v>
+        <v>69.7</v>
       </c>
       <c r="Q35">
-        <v>49.8</v>
+        <v>70.2</v>
       </c>
       <c r="R35">
-        <v>14</v>
+        <v>25.6</v>
       </c>
       <c r="S35">
-        <v>6.7</v>
+        <v>11.6</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="B36" s="1">
         <v>45125</v>
@@ -2747,7 +2818,7 @@
         <v>28</v>
       </c>
       <c r="D36">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E36">
         <v>4.0960000000000001</v>
@@ -2756,77 +2827,77 @@
         <v>4.0960000000000001</v>
       </c>
       <c r="G36">
-        <v>0.05</v>
+        <v>0.13</v>
       </c>
       <c r="H36">
-        <v>0.05</v>
+        <v>0.13</v>
       </c>
       <c r="J36">
         <v>2000</v>
       </c>
       <c r="K36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P36">
-        <v>45.7</v>
+        <v>53.8</v>
       </c>
       <c r="Q36">
-        <v>37.9</v>
+        <v>49.8</v>
       </c>
       <c r="R36">
-        <v>7.9</v>
+        <v>14</v>
       </c>
       <c r="S36">
-        <v>3.8</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="B37" s="1">
-        <v>45400</v>
+        <v>45125</v>
       </c>
       <c r="C37" t="s">
         <v>28</v>
       </c>
       <c r="D37">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E37">
-        <v>8.1920000000000002</v>
+        <v>4.0960000000000001</v>
       </c>
       <c r="F37">
-        <v>8.1920000000000002</v>
+        <v>4.0960000000000001</v>
       </c>
       <c r="G37">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H37">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="J37">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="K37" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="P37">
-        <v>68.400000000000006</v>
+        <v>45.7</v>
       </c>
       <c r="Q37">
-        <v>58.4</v>
+        <v>37.9</v>
       </c>
       <c r="R37">
-        <v>62.2</v>
+        <v>7.9</v>
       </c>
       <c r="S37">
-        <v>30</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B38" s="1">
         <v>45400</v>
@@ -2835,7 +2906,7 @@
         <v>28</v>
       </c>
       <c r="D38">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="E38">
         <v>8.1920000000000002</v>
@@ -2844,77 +2915,86 @@
         <v>8.1920000000000002</v>
       </c>
       <c r="G38">
-        <v>0.59</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H38">
-        <v>0.79</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J38">
         <v>15000</v>
       </c>
       <c r="K38" t="s">
-        <v>76</v>
-      </c>
-      <c r="L38" t="b">
-        <v>1</v>
-      </c>
-      <c r="M38" t="b">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="P38">
-        <v>79.5</v>
+        <v>68.400000000000006</v>
       </c>
       <c r="Q38">
-        <v>79.7</v>
+        <v>58.4</v>
       </c>
       <c r="R38">
-        <v>81.7</v>
+        <v>62.2</v>
       </c>
       <c r="S38">
-        <v>50.4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="B39" s="1">
-        <v>44893</v>
+        <v>45400</v>
+      </c>
+      <c r="C39" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39">
+        <v>70</v>
       </c>
       <c r="E39">
-        <v>100</v>
+        <v>8.1920000000000002</v>
       </c>
       <c r="F39">
-        <v>4.0960000000000001</v>
+        <v>8.1920000000000002</v>
       </c>
       <c r="G39">
-        <v>8</v>
+        <v>0.59</v>
       </c>
       <c r="H39">
-        <v>24</v>
+        <v>0.79</v>
       </c>
       <c r="J39">
-        <v>400</v>
+        <v>15000</v>
       </c>
       <c r="K39" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="L39" t="b">
         <v>1</v>
       </c>
       <c r="M39" t="b">
         <v>1</v>
+      </c>
+      <c r="P39">
+        <v>79.5</v>
+      </c>
+      <c r="Q39">
+        <v>79.7</v>
+      </c>
+      <c r="R39">
+        <v>81.7</v>
+      </c>
+      <c r="S39">
+        <v>50.4</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B40" s="1">
-        <v>45118</v>
-      </c>
-      <c r="D40" t="s">
-        <v>83</v>
+        <v>44893</v>
       </c>
       <c r="E40">
         <v>100</v>
@@ -2928,31 +3008,31 @@
       <c r="H40">
         <v>24</v>
       </c>
+      <c r="J40">
+        <v>400</v>
+      </c>
+      <c r="K40" t="s">
+        <v>26</v>
+      </c>
       <c r="L40" t="b">
         <v>1</v>
       </c>
       <c r="M40" t="b">
         <v>1</v>
-      </c>
-      <c r="P40">
-        <v>75</v>
-      </c>
-      <c r="R40">
-        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B41" s="1">
-        <v>45253</v>
+        <v>45118</v>
       </c>
       <c r="D41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E41">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F41">
         <v>4.0960000000000001</v>
@@ -2969,16 +3049,22 @@
       <c r="M41" t="b">
         <v>1</v>
       </c>
+      <c r="P41">
+        <v>75</v>
+      </c>
+      <c r="R41">
+        <v>70</v>
+      </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="B42" s="1">
-        <v>45355</v>
+        <v>45253</v>
       </c>
       <c r="D42" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E42">
         <v>200</v>
@@ -2987,40 +3073,16 @@
         <v>4.0960000000000001</v>
       </c>
       <c r="G42">
-        <v>0.25</v>
+        <v>8</v>
       </c>
       <c r="H42">
-        <v>1.25</v>
-      </c>
-      <c r="I42">
-        <v>0.4</v>
+        <v>24</v>
       </c>
       <c r="L42" t="b">
         <v>1</v>
       </c>
       <c r="M42" t="b">
         <v>1</v>
-      </c>
-      <c r="N42" t="b">
-        <v>1</v>
-      </c>
-      <c r="P42">
-        <v>75.2</v>
-      </c>
-      <c r="Q42">
-        <v>78.400000000000006</v>
-      </c>
-      <c r="R42">
-        <v>75.900000000000006</v>
-      </c>
-      <c r="S42">
-        <v>38.9</v>
-      </c>
-      <c r="T42">
-        <v>50.2</v>
-      </c>
-      <c r="U42">
-        <v>46.4</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
@@ -3031,7 +3093,7 @@
         <v>45355</v>
       </c>
       <c r="D43" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E43">
         <v>200</v>
@@ -3040,45 +3102,45 @@
         <v>4.0960000000000001</v>
       </c>
       <c r="G43">
-        <v>3</v>
+        <v>0.25</v>
       </c>
       <c r="H43">
-        <v>15</v>
+        <v>1.25</v>
       </c>
       <c r="I43">
-        <v>4.8</v>
+        <v>0.4</v>
       </c>
       <c r="N43" t="b">
         <v>1</v>
       </c>
       <c r="P43">
-        <v>79</v>
+        <v>75.2</v>
       </c>
       <c r="Q43">
-        <v>78.900000000000006</v>
+        <v>78.400000000000006</v>
       </c>
       <c r="R43">
-        <v>73</v>
+        <v>75.900000000000006</v>
       </c>
       <c r="S43">
-        <v>43.1</v>
+        <v>38.9</v>
       </c>
       <c r="T43">
-        <v>53.1</v>
+        <v>50.2</v>
       </c>
       <c r="U43">
-        <v>47.9</v>
+        <v>46.4</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B44" s="1">
         <v>45355</v>
       </c>
       <c r="D44" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="E44">
         <v>200</v>
@@ -3087,244 +3149,274 @@
         <v>4.0960000000000001</v>
       </c>
       <c r="G44">
+        <v>3</v>
+      </c>
+      <c r="H44">
         <v>15</v>
       </c>
-      <c r="H44">
-        <v>75</v>
-      </c>
       <c r="I44">
-        <v>24</v>
+        <v>4.8</v>
       </c>
       <c r="N44" t="b">
         <v>1</v>
       </c>
       <c r="P44">
-        <v>86.8</v>
+        <v>79</v>
       </c>
       <c r="Q44">
-        <v>83.1</v>
+        <v>78.900000000000006</v>
       </c>
       <c r="R44">
-        <v>84.9</v>
+        <v>73</v>
       </c>
       <c r="S44">
-        <v>60.1</v>
+        <v>43.1</v>
       </c>
       <c r="T44">
-        <v>59.4</v>
+        <v>53.1</v>
       </c>
       <c r="U44">
-        <v>50.5</v>
+        <v>47.9</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B45" s="1">
-        <v>45260</v>
-      </c>
-      <c r="C45" t="s">
-        <v>42</v>
-      </c>
-      <c r="D45">
-        <v>1.8</v>
+        <v>45355</v>
+      </c>
+      <c r="D45" t="s">
+        <v>116</v>
       </c>
       <c r="E45">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="F45">
-        <v>2</v>
+        <v>4.0960000000000001</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="K45" t="s">
-        <v>43</v>
+        <v>75</v>
+      </c>
+      <c r="I45">
+        <v>24</v>
+      </c>
+      <c r="L45" t="b">
+        <v>1</v>
+      </c>
+      <c r="M45" t="b">
+        <v>1</v>
+      </c>
+      <c r="N45" t="b">
+        <v>1</v>
       </c>
       <c r="P45">
-        <v>45.3</v>
+        <v>86.8</v>
+      </c>
+      <c r="Q45">
+        <v>83.1</v>
       </c>
       <c r="R45">
-        <v>15.2</v>
+        <v>84.9</v>
       </c>
       <c r="S45">
-        <v>2.2999999999999998</v>
+        <v>60.1</v>
+      </c>
+      <c r="T45">
+        <v>59.4</v>
+      </c>
+      <c r="U45">
+        <v>50.5</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>41</v>
+        <v>129</v>
       </c>
       <c r="B46" s="1">
-        <v>45141</v>
+        <v>45463</v>
       </c>
       <c r="C46" t="s">
-        <v>42</v>
-      </c>
-      <c r="D46">
-        <v>7</v>
+        <v>146</v>
+      </c>
+      <c r="D46" t="s">
+        <v>84</v>
       </c>
       <c r="E46">
-        <v>6</v>
+        <v>200</v>
       </c>
       <c r="F46">
-        <v>2</v>
+        <v>8.1920000000000002</v>
       </c>
       <c r="G46">
-        <v>0.85</v>
+        <v>3</v>
       </c>
       <c r="H46">
-        <v>0.85</v>
+        <v>15</v>
+      </c>
+      <c r="I46">
+        <v>4.8</v>
       </c>
       <c r="K46" t="s">
-        <v>43</v>
+        <v>20</v>
+      </c>
+      <c r="L46" t="b">
+        <v>1</v>
+      </c>
+      <c r="M46" t="b">
+        <v>1</v>
+      </c>
+      <c r="N46" t="b">
+        <v>1</v>
       </c>
       <c r="P46">
-        <v>58.2</v>
+        <v>88.7</v>
+      </c>
+      <c r="Q46">
+        <v>87.1</v>
       </c>
       <c r="R46">
-        <v>31.6</v>
+        <v>92</v>
       </c>
       <c r="S46">
-        <v>11.6</v>
+        <v>71.099999999999994</v>
+      </c>
+      <c r="T46">
+        <v>67.7</v>
+      </c>
+      <c r="U46">
+        <v>68.3</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B47" s="1">
-        <v>45194</v>
+        <v>45260</v>
       </c>
       <c r="C47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D47">
-        <v>14</v>
+        <v>1.8</v>
       </c>
       <c r="E47">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F47">
         <v>2</v>
       </c>
       <c r="G47">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="H47">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="K47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P47">
-        <v>66.3</v>
+        <v>45.3</v>
       </c>
       <c r="R47">
-        <v>40.799999999999997</v>
+        <v>15.2</v>
       </c>
       <c r="S47">
-        <v>24.8</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B48" s="1">
-        <v>45260</v>
+        <v>45141</v>
       </c>
       <c r="C48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D48">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="E48">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="F48">
         <v>2</v>
       </c>
       <c r="G48">
-        <v>2.8</v>
+        <v>0.85</v>
       </c>
       <c r="H48">
-        <v>2.8</v>
+        <v>0.85</v>
       </c>
       <c r="K48" t="s">
-        <v>43</v>
-      </c>
-      <c r="L48" t="b">
-        <v>1</v>
-      </c>
-      <c r="M48" t="b">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="P48">
-        <v>77.400000000000006</v>
+        <v>58.2</v>
       </c>
       <c r="R48">
-        <v>52.2</v>
+        <v>31.6</v>
       </c>
       <c r="S48">
-        <v>35.200000000000003</v>
+        <v>11.6</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="B49" s="1">
-        <v>45328</v>
+        <v>45194</v>
       </c>
       <c r="C49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D49">
-        <v>0.5</v>
+        <v>14</v>
       </c>
       <c r="E49">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="F49">
         <v>2</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P49">
-        <v>39.200000000000003</v>
+        <v>66.3</v>
       </c>
       <c r="R49">
-        <v>12.2</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="S49">
-        <v>3.1</v>
+        <v>24.8</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B50" s="1">
-        <v>45328</v>
+        <v>45260</v>
       </c>
       <c r="C50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D50">
-        <v>1.8</v>
+        <v>72</v>
       </c>
       <c r="E50">
         <v>30</v>
@@ -3333,191 +3425,194 @@
         <v>2</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="H50">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="K50" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="L50" t="b">
+        <v>1</v>
+      </c>
+      <c r="M50" t="b">
+        <v>1</v>
       </c>
       <c r="P50">
-        <v>46.8</v>
+        <v>77.400000000000006</v>
       </c>
       <c r="R50">
-        <v>20.100000000000001</v>
+        <v>52.2</v>
       </c>
       <c r="S50">
-        <v>10.1</v>
+        <v>35.200000000000003</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B51" s="1">
         <v>45328</v>
       </c>
       <c r="C51" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D51">
-        <v>7</v>
+        <v>0.5</v>
       </c>
       <c r="E51">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F51">
         <v>2</v>
       </c>
       <c r="G51">
-        <v>0.14000000000000001</v>
+        <v>0</v>
       </c>
       <c r="H51">
-        <v>0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="K51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P51">
-        <v>61</v>
+        <v>39.200000000000003</v>
       </c>
       <c r="R51">
-        <v>36</v>
+        <v>12.2</v>
       </c>
       <c r="S51">
-        <v>20.3</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B52" s="1">
         <v>45328</v>
       </c>
       <c r="C52" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D52">
-        <v>14</v>
+        <v>1.8</v>
       </c>
       <c r="E52">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F52">
         <v>2</v>
       </c>
       <c r="G52">
-        <v>0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="H52">
-        <v>0.56000000000000005</v>
+        <v>0</v>
       </c>
       <c r="K52" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P52">
-        <v>67.599999999999994</v>
+        <v>46.8</v>
       </c>
       <c r="R52">
-        <v>37.799999999999997</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="S52">
-        <v>29.2</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B53" s="1">
         <v>45328</v>
       </c>
       <c r="C53" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D53">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="E53">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="F53">
         <v>2</v>
       </c>
       <c r="G53">
-        <v>0.49</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H53">
-        <v>0.98</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="K53" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P53">
-        <v>73.400000000000006</v>
+        <v>61</v>
       </c>
       <c r="R53">
-        <v>37.200000000000003</v>
+        <v>36</v>
       </c>
       <c r="S53">
-        <v>36.1</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B54" s="1">
         <v>45328</v>
       </c>
       <c r="C54" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D54">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="E54">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="F54">
         <v>2</v>
       </c>
       <c r="G54">
-        <v>0.7</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H54">
-        <v>1.4</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="K54" t="s">
-        <v>43</v>
-      </c>
-      <c r="L54" t="b">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="P54">
-        <v>77.5</v>
+        <v>67.599999999999994</v>
       </c>
       <c r="R54">
-        <v>41.5</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="S54">
-        <v>34.1</v>
+        <v>29.2</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B55" s="1">
-        <v>45402</v>
+        <v>45328</v>
       </c>
       <c r="C55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D55">
-        <v>110</v>
+        <v>32</v>
       </c>
       <c r="E55">
         <v>30</v>
@@ -3526,68 +3621,77 @@
         <v>2</v>
       </c>
       <c r="G55">
+        <v>0.49</v>
+      </c>
+      <c r="H55">
         <v>0.98</v>
       </c>
-      <c r="H55">
-        <v>1.96</v>
-      </c>
       <c r="K55" t="s">
-        <v>43</v>
-      </c>
-      <c r="M55" t="b">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="P55">
-        <v>80.400000000000006</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="R55">
-        <v>52.4</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="S55">
-        <v>49.6</v>
+        <v>36.1</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="B56" s="1">
-        <v>45027</v>
+        <v>45328</v>
       </c>
       <c r="C56" t="s">
-        <v>42</v>
-      </c>
-      <c r="D56" t="s">
-        <v>107</v>
+        <v>41</v>
+      </c>
+      <c r="D56">
+        <v>72</v>
       </c>
       <c r="E56">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F56">
         <v>2</v>
       </c>
       <c r="G56">
-        <v>0.28000000000000003</v>
+        <v>0.7</v>
       </c>
       <c r="H56">
-        <v>0.84</v>
+        <v>1.4</v>
       </c>
       <c r="K56" t="s">
-        <v>20</v>
+        <v>42</v>
+      </c>
+      <c r="L56" t="b">
+        <v>1</v>
+      </c>
+      <c r="P56">
+        <v>77.5</v>
+      </c>
+      <c r="R56">
+        <v>41.5</v>
+      </c>
+      <c r="S56">
+        <v>34.1</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="B57" s="1">
-        <v>45027</v>
+        <v>45402</v>
       </c>
       <c r="C57" t="s">
-        <v>42</v>
-      </c>
-      <c r="D57" t="s">
-        <v>107</v>
+        <v>41</v>
+      </c>
+      <c r="D57">
+        <v>110</v>
       </c>
       <c r="E57">
         <v>30</v>
@@ -3596,33 +3700,39 @@
         <v>2</v>
       </c>
       <c r="G57">
-        <v>0.56000000000000005</v>
+        <v>0.98</v>
       </c>
       <c r="H57">
-        <v>1.68</v>
+        <v>1.96</v>
       </c>
       <c r="K57" t="s">
-        <v>20</v>
-      </c>
-      <c r="L57" t="b">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="M57" t="b">
         <v>1</v>
+      </c>
+      <c r="P57">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="R57">
+        <v>52.4</v>
+      </c>
+      <c r="S57">
+        <v>49.6</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B58" s="1">
-        <v>45261</v>
+        <v>45027</v>
       </c>
       <c r="C58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D58" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E58">
         <v>6</v>
@@ -3631,59 +3741,62 @@
         <v>2</v>
       </c>
       <c r="G58">
-        <v>16.8</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H58">
-        <v>16.8</v>
+        <v>0.84</v>
       </c>
       <c r="K58" t="s">
         <v>20</v>
       </c>
-      <c r="L58" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B59" s="1">
-        <v>45298</v>
+        <v>45027</v>
       </c>
       <c r="C59" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D59" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E59">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F59">
         <v>2</v>
       </c>
       <c r="G59">
-        <v>5.6</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H59">
-        <v>16.8</v>
+        <v>1.68</v>
       </c>
       <c r="K59" t="s">
         <v>20</v>
       </c>
+      <c r="L59" t="b">
+        <v>1</v>
+      </c>
+      <c r="M59" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B60" s="1">
-        <v>45385</v>
+        <v>45261</v>
       </c>
       <c r="C60" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D60" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E60">
         <v>6</v>
@@ -3692,7 +3805,7 @@
         <v>2</v>
       </c>
       <c r="G60">
-        <v>5.6</v>
+        <v>16.8</v>
       </c>
       <c r="H60">
         <v>16.8</v>
@@ -3700,7 +3813,7 @@
       <c r="K60" t="s">
         <v>20</v>
       </c>
-      <c r="M60" t="b">
+      <c r="L60" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3709,13 +3822,13 @@
         <v>102</v>
       </c>
       <c r="B61" s="1">
-        <v>45410</v>
+        <v>45298</v>
       </c>
       <c r="C61" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D61" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E61">
         <v>6</v>
@@ -3732,60 +3845,51 @@
       <c r="K61" t="s">
         <v>20</v>
       </c>
-      <c r="L61" t="b">
-        <v>1</v>
-      </c>
-      <c r="M61" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="B62" s="1">
-        <v>45433</v>
+        <v>45385</v>
       </c>
       <c r="C62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D62" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E62">
-        <v>10000</v>
+        <v>6</v>
       </c>
       <c r="F62">
         <v>2</v>
       </c>
       <c r="G62">
-        <v>7.0000000000000007E-2</v>
+        <v>5.6</v>
       </c>
       <c r="H62">
-        <v>0.28000000000000003</v>
+        <v>16.8</v>
       </c>
       <c r="K62" t="s">
         <v>20</v>
       </c>
-      <c r="L62" t="b">
-        <v>1</v>
-      </c>
       <c r="M62" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="B63" s="1">
-        <v>45217</v>
+        <v>45410</v>
       </c>
       <c r="C63" t="s">
-        <v>42</v>
-      </c>
-      <c r="D63">
-        <v>7</v>
+        <v>41</v>
+      </c>
+      <c r="D63" t="s">
+        <v>99</v>
       </c>
       <c r="E63">
         <v>6</v>
@@ -3794,77 +3898,68 @@
         <v>2</v>
       </c>
       <c r="G63">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="H63">
-        <v>0</v>
-      </c>
-      <c r="I63">
-        <v>0</v>
+        <v>16.8</v>
       </c>
       <c r="K63" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="L63" t="b">
         <v>1</v>
       </c>
-      <c r="N63" t="b">
-        <v>1</v>
-      </c>
-      <c r="P63">
-        <v>58.2</v>
-      </c>
-      <c r="R63">
-        <v>31.6</v>
-      </c>
-      <c r="S63">
-        <v>11.6</v>
+      <c r="M63" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="B64" s="1">
-        <v>45261</v>
+        <v>45433</v>
       </c>
       <c r="C64" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D64" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E64">
-        <v>6</v>
+        <v>10000</v>
       </c>
       <c r="F64">
         <v>2</v>
       </c>
       <c r="G64">
-        <v>1.1000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H64">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I64">
-        <v>1.4</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="K64" t="s">
         <v>20</v>
       </c>
+      <c r="L64" t="b">
+        <v>1</v>
+      </c>
+      <c r="M64" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="B65" s="1">
-        <v>45261</v>
+        <v>45217</v>
       </c>
       <c r="C65" t="s">
-        <v>42</v>
-      </c>
-      <c r="D65" t="s">
-        <v>101</v>
+        <v>41</v>
+      </c>
+      <c r="D65">
+        <v>7</v>
       </c>
       <c r="E65">
         <v>6</v>
@@ -3873,316 +3968,375 @@
         <v>2</v>
       </c>
       <c r="G65">
-        <v>2.8</v>
+        <v>0</v>
       </c>
       <c r="H65">
-        <v>2.8</v>
+        <v>0</v>
       </c>
       <c r="I65">
-        <v>3.6</v>
+        <v>0</v>
       </c>
       <c r="K65" t="s">
-        <v>20</v>
-      </c>
-      <c r="M65" t="b">
+        <v>42</v>
+      </c>
+      <c r="L65" t="b">
         <v>1</v>
       </c>
       <c r="N65" t="b">
         <v>1</v>
+      </c>
+      <c r="P65">
+        <v>58.2</v>
+      </c>
+      <c r="R65">
+        <v>31.6</v>
+      </c>
+      <c r="S65">
+        <v>11.6</v>
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
       <c r="B66" s="1">
-        <v>45196</v>
+        <v>45261</v>
+      </c>
+      <c r="C66" t="s">
+        <v>41</v>
+      </c>
+      <c r="D66" t="s">
+        <v>99</v>
       </c>
       <c r="E66">
-        <v>32.768000000000001</v>
+        <v>6</v>
       </c>
       <c r="F66">
-        <v>32.768000000000001</v>
+        <v>2</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H66">
-        <v>0</v>
-      </c>
-      <c r="L66" t="b">
-        <v>1</v>
-      </c>
-      <c r="M66" t="b">
-        <v>1</v>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I66">
+        <v>1.4</v>
+      </c>
+      <c r="K66" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="B67" s="1">
-        <v>45271</v>
+        <v>45261</v>
+      </c>
+      <c r="C67" t="s">
+        <v>41</v>
+      </c>
+      <c r="D67" t="s">
+        <v>99</v>
       </c>
       <c r="E67">
-        <v>32.768000000000001</v>
+        <v>6</v>
       </c>
       <c r="F67">
-        <v>32.768000000000001</v>
+        <v>2</v>
       </c>
       <c r="G67">
-        <v>0.24</v>
+        <v>2.8</v>
       </c>
       <c r="H67">
-        <v>0.24</v>
-      </c>
-      <c r="L67" t="b">
-        <v>1</v>
+        <v>2.8</v>
+      </c>
+      <c r="I67">
+        <v>3.6</v>
+      </c>
+      <c r="K67" t="s">
+        <v>20</v>
       </c>
       <c r="M67" t="b">
+        <v>1</v>
+      </c>
+      <c r="N67" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>68</v>
+        <v>139</v>
       </c>
       <c r="B68" s="1">
-        <v>45348</v>
+        <v>45450</v>
       </c>
       <c r="C68" t="s">
-        <v>81</v>
-      </c>
-      <c r="D68" t="s">
-        <v>82</v>
+        <v>41</v>
+      </c>
+      <c r="D68">
+        <v>0.5</v>
       </c>
       <c r="E68">
         <v>32</v>
       </c>
       <c r="F68">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="G68">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H68">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="K68" t="s">
-        <v>20</v>
-      </c>
-      <c r="L68" t="b">
-        <v>1</v>
-      </c>
-      <c r="M68" t="b">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="P68">
-        <v>81.2</v>
+        <v>45.4</v>
       </c>
       <c r="R68">
-        <v>45.1</v>
+        <v>22</v>
       </c>
       <c r="S68">
-        <v>45</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>69</v>
+        <v>140</v>
       </c>
       <c r="B69" s="1">
-        <v>45348</v>
+        <v>45450</v>
       </c>
       <c r="C69" t="s">
-        <v>47</v>
-      </c>
-      <c r="D69" t="s">
-        <v>119</v>
+        <v>41</v>
+      </c>
+      <c r="D69">
+        <v>1.5</v>
       </c>
       <c r="E69">
         <v>32</v>
       </c>
       <c r="F69">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="G69">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="H69">
-        <v>8.1</v>
+        <v>0</v>
       </c>
       <c r="K69" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="P69">
+        <v>56.5</v>
+      </c>
+      <c r="R69">
+        <v>31.1</v>
+      </c>
+      <c r="S69">
+        <v>21.7</v>
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B70" s="1"/>
-      <c r="J70">
-        <v>4000</v>
-      </c>
-      <c r="L70" t="b">
-        <v>1</v>
-      </c>
-      <c r="M70" t="b">
-        <v>1</v>
+        <v>141</v>
+      </c>
+      <c r="B70" s="1">
+        <v>45450</v>
+      </c>
+      <c r="C70" t="s">
+        <v>41</v>
+      </c>
+      <c r="D70">
+        <v>7</v>
+      </c>
+      <c r="E70">
+        <v>128</v>
+      </c>
+      <c r="F70">
+        <v>2</v>
+      </c>
+      <c r="G70">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H70">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K70" t="s">
+        <v>16</v>
+      </c>
+      <c r="P70">
+        <v>70.3</v>
+      </c>
+      <c r="R70">
+        <v>51.2</v>
+      </c>
+      <c r="S70">
+        <v>44.2</v>
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>36</v>
+        <v>142</v>
       </c>
       <c r="B71" s="1">
-        <v>45104</v>
+        <v>45450</v>
       </c>
       <c r="C71" t="s">
-        <v>22</v>
-      </c>
-      <c r="D71" t="s">
-        <v>84</v>
+        <v>41</v>
+      </c>
+      <c r="D71">
+        <v>57</v>
       </c>
       <c r="E71">
-        <v>8.1920000000000002</v>
+        <v>64</v>
       </c>
       <c r="F71">
-        <v>8.1920000000000002</v>
+        <v>2</v>
       </c>
       <c r="G71">
-        <v>1.7</v>
+        <v>0.49</v>
       </c>
       <c r="H71">
-        <v>1.7</v>
+        <v>0.98</v>
       </c>
       <c r="K71" t="s">
-        <v>20</v>
-      </c>
-      <c r="L71" t="b">
-        <v>1</v>
-      </c>
-      <c r="M71" t="b">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="P71">
+        <v>76.5</v>
+      </c>
+      <c r="R71">
+        <v>53</v>
+      </c>
+      <c r="S71">
+        <v>43</v>
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>74</v>
+        <v>143</v>
       </c>
       <c r="B72" s="1">
-        <v>45398</v>
+        <v>45450</v>
       </c>
       <c r="C72" t="s">
-        <v>22</v>
-      </c>
-      <c r="D72" t="s">
-        <v>85</v>
+        <v>41</v>
+      </c>
+      <c r="D72">
+        <v>72</v>
       </c>
       <c r="E72">
-        <v>8.1920000000000002</v>
+        <v>128</v>
       </c>
       <c r="F72">
-        <v>8.1920000000000002</v>
+        <v>2</v>
       </c>
       <c r="G72">
-        <v>2.1</v>
+        <v>0.7</v>
       </c>
       <c r="H72">
-        <v>4.2</v>
+        <v>1.4</v>
       </c>
       <c r="K72" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="L72" t="b">
         <v>1</v>
       </c>
       <c r="M72" t="b">
         <v>1</v>
+      </c>
+      <c r="P72">
+        <v>84.2</v>
+      </c>
+      <c r="R72">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="S72">
+        <v>51.1</v>
       </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B73" s="1">
-        <v>45246</v>
-      </c>
-      <c r="C73" t="s">
-        <v>52</v>
-      </c>
-      <c r="D73" t="s">
-        <v>86</v>
+        <v>45196</v>
       </c>
       <c r="E73">
-        <v>32</v>
+        <v>32.768000000000001</v>
       </c>
       <c r="F73">
-        <v>32</v>
+        <v>32.768000000000001</v>
       </c>
       <c r="G73">
-        <v>3.4</v>
+        <v>0</v>
       </c>
       <c r="H73">
-        <v>3.4</v>
-      </c>
-      <c r="K73" t="s">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="L73" t="b">
+        <v>1</v>
+      </c>
+      <c r="M73" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B74" s="1">
-        <v>45246</v>
-      </c>
-      <c r="C74" t="s">
-        <v>52</v>
-      </c>
-      <c r="D74" t="s">
-        <v>86</v>
+        <v>45271</v>
       </c>
       <c r="E74">
-        <v>8</v>
+        <v>32.768000000000001</v>
       </c>
       <c r="F74">
-        <v>8</v>
+        <v>32.768000000000001</v>
       </c>
       <c r="G74">
-        <v>1.7</v>
+        <v>0.24</v>
       </c>
       <c r="H74">
-        <v>1.7</v>
-      </c>
-      <c r="K74" t="s">
-        <v>20</v>
+        <v>0.24</v>
+      </c>
+      <c r="L74" t="b">
+        <v>1</v>
+      </c>
+      <c r="M74" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B75" s="1">
-        <v>45246</v>
+        <v>45348</v>
       </c>
       <c r="C75" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="D75" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E75">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="F75">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="G75">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="H75">
-        <v>8.5</v>
+        <v>24</v>
       </c>
       <c r="K75" t="s">
         <v>20</v>
@@ -4193,48 +4347,52 @@
       <c r="M75" t="b">
         <v>1</v>
       </c>
+      <c r="P75">
+        <v>81.2</v>
+      </c>
+      <c r="R75">
+        <v>45.1</v>
+      </c>
+      <c r="S75">
+        <v>45</v>
+      </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="B76" s="1">
-        <v>45234</v>
-      </c>
-      <c r="L76" t="b">
-        <v>1</v>
-      </c>
-      <c r="M76" t="b">
-        <v>1</v>
-      </c>
-      <c r="P76">
-        <v>73</v>
-      </c>
-      <c r="R76">
-        <v>63.2</v>
-      </c>
-      <c r="S76">
-        <v>23.9</v>
+        <v>45348</v>
+      </c>
+      <c r="C76" t="s">
+        <v>45</v>
+      </c>
+      <c r="D76" t="s">
+        <v>117</v>
+      </c>
+      <c r="E76">
+        <v>32</v>
+      </c>
+      <c r="F76">
+        <v>32</v>
+      </c>
+      <c r="G76">
+        <v>2.7</v>
+      </c>
+      <c r="H76">
+        <v>8.1</v>
+      </c>
+      <c r="K76" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B77" s="1">
-        <v>44986</v>
-      </c>
-      <c r="C77" t="s">
-        <v>29</v>
-      </c>
-      <c r="D77">
-        <v>1085</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B77" s="1"/>
       <c r="J77">
-        <v>329</v>
-      </c>
-      <c r="K77" t="s">
-        <v>20</v>
+        <v>4000</v>
       </c>
       <c r="L77" t="b">
         <v>1</v>
@@ -4245,28 +4403,28 @@
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>122</v>
+        <v>36</v>
       </c>
       <c r="B78" s="1">
-        <v>45425</v>
+        <v>45104</v>
       </c>
       <c r="C78" t="s">
-        <v>123</v>
+        <v>22</v>
       </c>
       <c r="D78" t="s">
-        <v>124</v>
+        <v>82</v>
       </c>
       <c r="E78">
-        <v>16</v>
+        <v>8.1920000000000002</v>
       </c>
       <c r="F78">
-        <v>16</v>
+        <v>8.1920000000000002</v>
       </c>
       <c r="G78">
-        <v>2.8</v>
+        <v>1.7</v>
       </c>
       <c r="H78">
-        <v>2.8</v>
+        <v>1.7</v>
       </c>
       <c r="K78" t="s">
         <v>20</v>
@@ -4277,310 +4435,602 @@
       <c r="M78" t="b">
         <v>1</v>
       </c>
-      <c r="P78">
-        <v>83.8</v>
-      </c>
-      <c r="R78">
-        <v>82.3</v>
-      </c>
-      <c r="S78">
-        <v>62.4</v>
-      </c>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>125</v>
+        <v>72</v>
       </c>
       <c r="B79" s="1">
-        <v>45425</v>
+        <v>45398</v>
       </c>
       <c r="C79" t="s">
-        <v>123</v>
+        <v>22</v>
       </c>
       <c r="D79" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="E79">
-        <v>16</v>
+        <v>8.1920000000000002</v>
       </c>
       <c r="F79">
-        <v>16</v>
+        <v>8.1920000000000002</v>
       </c>
       <c r="G79">
-        <v>0.35</v>
+        <v>2.1</v>
       </c>
       <c r="H79">
-        <v>0.35</v>
+        <v>4.2</v>
       </c>
       <c r="K79" t="s">
         <v>20</v>
       </c>
-      <c r="P79">
-        <v>76.8</v>
-      </c>
-      <c r="R79">
-        <v>75.2</v>
-      </c>
-      <c r="S79">
-        <v>50.1</v>
+      <c r="L79" t="b">
+        <v>1</v>
+      </c>
+      <c r="M79" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>127</v>
+        <v>49</v>
       </c>
       <c r="B80" s="1">
-        <v>45307</v>
+        <v>45246</v>
       </c>
       <c r="C80" t="s">
-        <v>128</v>
+        <v>50</v>
       </c>
       <c r="D80" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E80">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="F80">
-        <v>8.1920000000000002</v>
+        <v>32</v>
       </c>
       <c r="G80">
-        <v>14.1</v>
+        <v>3.4</v>
       </c>
       <c r="H80">
-        <v>14.1</v>
+        <v>3.4</v>
       </c>
       <c r="K80" t="s">
         <v>20</v>
       </c>
-      <c r="L80" t="b">
-        <v>1</v>
-      </c>
-      <c r="M80" t="b">
-        <v>1</v>
-      </c>
-      <c r="P80">
-        <v>81.5</v>
-      </c>
-      <c r="R80">
-        <v>72</v>
-      </c>
-      <c r="S80">
-        <v>47.9</v>
-      </c>
-    </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>129</v>
+        <v>51</v>
       </c>
       <c r="B81" s="1">
-        <v>45307</v>
+        <v>45246</v>
       </c>
       <c r="C81" t="s">
-        <v>128</v>
+        <v>50</v>
       </c>
       <c r="D81" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E81">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F81">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G81">
-        <v>14.1</v>
+        <v>1.7</v>
       </c>
       <c r="H81">
-        <v>14.1</v>
-      </c>
-      <c r="I81">
-        <v>14.8</v>
+        <v>1.7</v>
       </c>
       <c r="K81" t="s">
         <v>20</v>
       </c>
-      <c r="L81" t="b">
-        <v>1</v>
-      </c>
-      <c r="M81" t="b">
-        <v>1</v>
-      </c>
-      <c r="N81" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B82" s="1">
-        <v>45450</v>
+        <v>45246</v>
       </c>
       <c r="C82" t="s">
-        <v>42</v>
-      </c>
-      <c r="D82">
-        <v>0.5</v>
+        <v>50</v>
+      </c>
+      <c r="D82" t="s">
+        <v>84</v>
       </c>
       <c r="E82">
-        <v>32</v>
+        <v>128</v>
       </c>
       <c r="F82">
+        <v>128</v>
+      </c>
+      <c r="G82">
+        <v>8.5</v>
+      </c>
+      <c r="H82">
+        <v>8.5</v>
+      </c>
+      <c r="K82" t="s">
+        <v>20</v>
+      </c>
+      <c r="L82" t="b">
+        <v>1</v>
+      </c>
+      <c r="M82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B83" s="1">
+        <v>45234</v>
+      </c>
+      <c r="L83" t="b">
+        <v>1</v>
+      </c>
+      <c r="M83" t="b">
+        <v>1</v>
+      </c>
+      <c r="P83">
+        <v>73</v>
+      </c>
+      <c r="R83">
+        <v>63.2</v>
+      </c>
+      <c r="S83">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B84" s="1">
+        <v>44986</v>
+      </c>
+      <c r="C84" t="s">
+        <v>29</v>
+      </c>
+      <c r="D84">
+        <v>1085</v>
+      </c>
+      <c r="J84">
+        <v>329</v>
+      </c>
+      <c r="K84" t="s">
+        <v>20</v>
+      </c>
+      <c r="L84" t="b">
+        <v>1</v>
+      </c>
+      <c r="M84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B85" s="1">
+        <v>45425</v>
+      </c>
+      <c r="C85" t="s">
+        <v>121</v>
+      </c>
+      <c r="D85" t="s">
+        <v>122</v>
+      </c>
+      <c r="E85">
+        <v>16</v>
+      </c>
+      <c r="F85">
+        <v>16</v>
+      </c>
+      <c r="G85">
+        <v>2.8</v>
+      </c>
+      <c r="H85">
+        <v>2.8</v>
+      </c>
+      <c r="K85" t="s">
+        <v>20</v>
+      </c>
+      <c r="L85" t="b">
+        <v>1</v>
+      </c>
+      <c r="M85" t="b">
+        <v>1</v>
+      </c>
+      <c r="P85">
+        <v>83.8</v>
+      </c>
+      <c r="R85">
+        <v>82.3</v>
+      </c>
+      <c r="S85">
+        <v>62.4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B86" s="1">
+        <v>45425</v>
+      </c>
+      <c r="C86" t="s">
+        <v>121</v>
+      </c>
+      <c r="D86" t="s">
+        <v>124</v>
+      </c>
+      <c r="E86">
+        <v>16</v>
+      </c>
+      <c r="F86">
+        <v>16</v>
+      </c>
+      <c r="G86">
+        <v>0.35</v>
+      </c>
+      <c r="H86">
+        <v>0.35</v>
+      </c>
+      <c r="K86" t="s">
+        <v>20</v>
+      </c>
+      <c r="P86">
+        <v>76.8</v>
+      </c>
+      <c r="R86">
+        <v>75.2</v>
+      </c>
+      <c r="S86">
+        <v>50.1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B87" s="1">
+        <v>45307</v>
+      </c>
+      <c r="C87" t="s">
+        <v>126</v>
+      </c>
+      <c r="D87" t="s">
+        <v>81</v>
+      </c>
+      <c r="E87">
+        <v>128</v>
+      </c>
+      <c r="F87">
+        <v>8.1920000000000002</v>
+      </c>
+      <c r="G87">
+        <v>14.1</v>
+      </c>
+      <c r="H87">
+        <v>14.1</v>
+      </c>
+      <c r="K87" t="s">
+        <v>20</v>
+      </c>
+      <c r="L87" t="b">
+        <v>1</v>
+      </c>
+      <c r="M87" t="b">
+        <v>1</v>
+      </c>
+      <c r="P87">
+        <v>81.5</v>
+      </c>
+      <c r="R87">
+        <v>72</v>
+      </c>
+      <c r="S87">
+        <v>47.9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B88" s="1">
+        <v>45307</v>
+      </c>
+      <c r="C88" t="s">
+        <v>126</v>
+      </c>
+      <c r="D88" t="s">
+        <v>81</v>
+      </c>
+      <c r="E88">
         <v>2</v>
       </c>
-      <c r="K82" t="s">
-        <v>16</v>
-      </c>
-      <c r="P82">
-        <v>45.4</v>
-      </c>
-      <c r="R82">
-        <v>22</v>
-      </c>
-      <c r="S82">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
+      <c r="F88">
+        <v>2</v>
+      </c>
+      <c r="G88">
+        <v>14.1</v>
+      </c>
+      <c r="H88">
+        <v>14.1</v>
+      </c>
+      <c r="I88">
+        <v>14.8</v>
+      </c>
+      <c r="K88" t="s">
+        <v>20</v>
+      </c>
+      <c r="L88" t="b">
+        <v>1</v>
+      </c>
+      <c r="M88" t="b">
+        <v>1</v>
+      </c>
+      <c r="N88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B83" s="1">
-        <v>45450</v>
-      </c>
-      <c r="C83" t="s">
-        <v>42</v>
-      </c>
-      <c r="D83">
-        <v>1.5</v>
-      </c>
-      <c r="E83">
-        <v>32</v>
-      </c>
-      <c r="F83">
-        <v>2</v>
-      </c>
-      <c r="K83" t="s">
-        <v>16</v>
-      </c>
-      <c r="P83">
-        <v>56.5</v>
-      </c>
-      <c r="R83">
-        <v>31.1</v>
-      </c>
-      <c r="S83">
-        <v>21.7</v>
-      </c>
-    </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B84" s="1">
-        <v>45450</v>
-      </c>
-      <c r="C84" t="s">
-        <v>42</v>
-      </c>
-      <c r="D84">
+      <c r="B89" s="1">
+        <v>45097</v>
+      </c>
+      <c r="C89" t="s">
+        <v>131</v>
+      </c>
+      <c r="D89">
+        <v>1.3</v>
+      </c>
+      <c r="E89">
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="F89">
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="J89">
         <v>7</v>
       </c>
-      <c r="E84">
+      <c r="K89" t="s">
+        <v>132</v>
+      </c>
+      <c r="L89" t="b">
+        <v>1</v>
+      </c>
+      <c r="M89" t="b">
+        <v>1</v>
+      </c>
+      <c r="R89">
+        <v>50.6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B90" s="1">
+        <v>45180</v>
+      </c>
+      <c r="C90" t="s">
+        <v>131</v>
+      </c>
+      <c r="D90">
+        <v>1.3</v>
+      </c>
+      <c r="E90">
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="F90">
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="J90">
+        <v>100</v>
+      </c>
+      <c r="K90" t="s">
+        <v>132</v>
+      </c>
+      <c r="L90" t="b">
+        <v>1</v>
+      </c>
+      <c r="M90" t="b">
+        <v>1</v>
+      </c>
+      <c r="P90">
+        <v>37.6</v>
+      </c>
+      <c r="R90">
+        <v>41.4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B91" s="1">
+        <v>45272</v>
+      </c>
+      <c r="C91" t="s">
+        <v>131</v>
+      </c>
+      <c r="D91">
+        <v>2.7</v>
+      </c>
+      <c r="E91">
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="F91">
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="J91">
+        <v>1400</v>
+      </c>
+      <c r="K91" t="s">
+        <v>132</v>
+      </c>
+      <c r="L91" t="b">
+        <v>1</v>
+      </c>
+      <c r="M91" t="b">
+        <v>1</v>
+      </c>
+      <c r="P91">
+        <v>56.7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B92" s="1">
+        <v>45405</v>
+      </c>
+      <c r="C92" t="s">
+        <v>131</v>
+      </c>
+      <c r="D92">
+        <v>3.8</v>
+      </c>
+      <c r="E92">
         <v>128</v>
       </c>
-      <c r="F84">
-        <v>2</v>
-      </c>
-      <c r="K84" t="s">
-        <v>16</v>
-      </c>
-      <c r="P84">
-        <v>70.3</v>
-      </c>
-      <c r="R84">
-        <v>51.2</v>
-      </c>
-      <c r="S84">
-        <v>44.2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+      <c r="F92">
+        <v>128</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="K92" t="s">
+        <v>132</v>
+      </c>
+      <c r="L92" t="b">
+        <v>1</v>
+      </c>
+      <c r="P92">
+        <v>68.8</v>
+      </c>
+      <c r="R92">
+        <v>59.1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B93" s="1">
+        <v>45433</v>
+      </c>
+      <c r="C93" t="s">
         <v>131</v>
       </c>
-      <c r="B85" s="1">
-        <v>45450</v>
-      </c>
-      <c r="C85" t="s">
-        <v>42</v>
-      </c>
-      <c r="D85">
-        <v>57</v>
-      </c>
-      <c r="E85">
-        <v>64</v>
-      </c>
-      <c r="F85">
-        <v>2</v>
-      </c>
-      <c r="K85" t="s">
-        <v>16</v>
-      </c>
-      <c r="P85">
-        <v>76.5</v>
-      </c>
-      <c r="R85">
-        <v>53</v>
-      </c>
-      <c r="S85">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
+      <c r="D93">
+        <v>7</v>
+      </c>
+      <c r="E93">
+        <v>128</v>
+      </c>
+      <c r="F93">
+        <v>128</v>
+      </c>
+      <c r="K93" t="s">
+        <v>132</v>
+      </c>
+      <c r="P93">
+        <v>75.7</v>
+      </c>
+      <c r="R93">
         <v>61</v>
       </c>
-      <c r="B86" s="1">
-        <v>45450</v>
-      </c>
-      <c r="C86" t="s">
-        <v>42</v>
-      </c>
-      <c r="D86">
-        <v>72</v>
-      </c>
-      <c r="E86">
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B94" s="1">
+        <v>45433</v>
+      </c>
+      <c r="C94" t="s">
+        <v>131</v>
+      </c>
+      <c r="D94">
+        <v>14</v>
+      </c>
+      <c r="E94">
         <v>128</v>
       </c>
-      <c r="F86">
-        <v>2</v>
-      </c>
-      <c r="K86" t="s">
-        <v>43</v>
-      </c>
-      <c r="L86" t="b">
-        <v>1</v>
-      </c>
-      <c r="M86" t="b">
-        <v>1</v>
-      </c>
-      <c r="P86">
-        <v>84.2</v>
-      </c>
-      <c r="R86">
-        <v>64.400000000000006</v>
-      </c>
-      <c r="S86">
-        <v>51.1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B91" s="1"/>
+      <c r="F94">
+        <v>128</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+      <c r="K94" t="s">
+        <v>132</v>
+      </c>
+      <c r="M94" t="b">
+        <v>1</v>
+      </c>
+      <c r="P94">
+        <v>78</v>
+      </c>
+      <c r="R94">
+        <v>62.2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B95" s="1">
+        <v>45433</v>
+      </c>
+      <c r="C95" t="s">
+        <v>131</v>
+      </c>
+      <c r="D95">
+        <v>4.2</v>
+      </c>
+      <c r="E95">
+        <v>128</v>
+      </c>
+      <c r="F95">
+        <v>128</v>
+      </c>
+      <c r="K95" t="s">
+        <v>132</v>
+      </c>
+      <c r="L95" t="b">
+        <v>1</v>
+      </c>
+      <c r="M95" t="b">
+        <v>1</v>
+      </c>
+      <c r="S95">
+        <v>40.4</v>
+      </c>
+      <c r="T95">
+        <v>44.5</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>